<commit_message>
Add lims job and bug fix
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20385"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mw\git\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50910C3-1D49-4FD5-A382-67C95A33D0BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2328C5B1-5611-442B-8699-027D56B8E0BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="7" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4203,12 +4203,6 @@
     <t>ECO-FLNTU-RTD</t>
   </si>
   <si>
-    <t>Klorofyllfluorescens</t>
-  </si>
-  <si>
-    <t>CHLFLUO_CTD</t>
-  </si>
-  <si>
     <t>0-50 µg/I</t>
   </si>
   <si>
@@ -4230,12 +4224,6 @@
     <t>ECO-FLPC-RTD</t>
   </si>
   <si>
-    <t>Phycocyaninfluorescens</t>
-  </si>
-  <si>
-    <t>PHYC_CTD</t>
-  </si>
-  <si>
     <t>0-230 ppb</t>
   </si>
   <si>
@@ -4450,6 +4438,18 @@
   </si>
   <si>
     <t>FLNTURTD-2288, FLNTURT-115</t>
+  </si>
+  <si>
+    <t>PHYC_CTD*</t>
+  </si>
+  <si>
+    <t>Phycocyaninfluorescens*</t>
+  </si>
+  <si>
+    <t>CHLFLUO_CTD*</t>
+  </si>
+  <si>
+    <t>Klorofyllfluorescens*</t>
   </si>
 </sst>
 </file>
@@ -47467,7 +47467,7 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -47493,7 +47493,7 @@
         <v>1099</v>
       </c>
       <c r="B1" s="345" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="C1" s="345" t="s">
         <v>390</v>
@@ -47520,7 +47520,7 @@
         <v>1106</v>
       </c>
       <c r="K1" s="345" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="L1" s="345" t="s">
         <v>1107</v>
@@ -47549,7 +47549,7 @@
         <v>1114</v>
       </c>
       <c r="B2" s="346" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="C2" s="346" t="s">
         <v>1115</v>
@@ -47576,7 +47576,7 @@
         <v>1122</v>
       </c>
       <c r="K2" s="346" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="L2" s="346" t="s">
         <v>1123</v>
@@ -47605,7 +47605,7 @@
         <v>1130</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="F3" s="348"/>
       <c r="G3" s="349"/>
@@ -47617,7 +47617,7 @@
         <v>1132</v>
       </c>
       <c r="K3" s="349" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="L3" s="89" t="s">
         <v>38</v>
@@ -47638,7 +47638,7 @@
         <v>1135</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>1136</v>
@@ -47665,7 +47665,7 @@
         <v>1143</v>
       </c>
       <c r="K4" s="349" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="N4" s="164" t="s">
         <v>1144</v>
@@ -47685,7 +47685,7 @@
         <v>1135</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>1136</v>
@@ -47712,7 +47712,7 @@
         <v>1143</v>
       </c>
       <c r="K5" s="349" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="N5" s="354"/>
       <c r="O5" s="355" t="s">
@@ -47733,7 +47733,7 @@
         <v>1152</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="F6" s="352" t="s">
         <v>1137</v>
@@ -47745,13 +47745,13 @@
         <v>1153</v>
       </c>
       <c r="I6" s="350" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="J6" s="357" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="K6" s="357" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="L6" s="358"/>
       <c r="M6" s="358"/>
@@ -47773,7 +47773,7 @@
         <v>1152</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="F7" s="352" t="s">
         <v>1137</v>
@@ -47785,13 +47785,13 @@
         <v>6164</v>
       </c>
       <c r="I7" s="350" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="J7" s="357" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="K7" s="357" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="L7" s="359"/>
       <c r="O7" s="359" t="s">
@@ -47815,19 +47815,19 @@
         <v>1159</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="F8" s="348"/>
       <c r="G8" s="349"/>
       <c r="H8" s="351"/>
       <c r="I8" s="350" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="J8" s="349" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="K8" s="349" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="L8" s="89" t="s">
         <v>38</v>
@@ -47850,7 +47850,7 @@
         <v>1163</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="F9" s="352" t="s">
         <v>1137</v>
@@ -47862,13 +47862,13 @@
         <v>1164</v>
       </c>
       <c r="I9" s="350" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="J9" s="349" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="K9" s="349" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="L9" s="352"/>
       <c r="M9" s="352"/>
@@ -47890,7 +47890,7 @@
         <v>1163</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="F10" s="352" t="s">
         <v>1137</v>
@@ -47902,13 +47902,13 @@
         <v>6164</v>
       </c>
       <c r="I10" s="350" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="J10" s="349" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="K10" s="349" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="L10" s="352"/>
       <c r="M10" s="359"/>
@@ -47927,10 +47927,10 @@
     </row>
     <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="F11" s="352" t="s">
         <v>1137</v>
@@ -47942,13 +47942,13 @@
         <v>1171</v>
       </c>
       <c r="I11" s="350" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="J11" s="349" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="K11" s="349" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="L11" s="352"/>
       <c r="M11" s="352"/>
@@ -47976,10 +47976,10 @@
       <c r="G12" s="349"/>
       <c r="H12" s="351"/>
       <c r="I12" s="350" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="K12" s="349" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="L12" s="89" t="s">
         <v>38</v>
@@ -47990,7 +47990,7 @@
         <v>1177</v>
       </c>
       <c r="B13" s="89" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="F13" s="352" t="s">
         <v>1178</v>
@@ -48008,7 +48008,7 @@
         <v>1181</v>
       </c>
       <c r="K13" s="349" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="L13" s="352"/>
       <c r="M13" s="352"/>
@@ -48021,10 +48021,10 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="89" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="B14" s="89" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="F14" s="89" t="s">
         <v>1184</v>
@@ -48033,25 +48033,25 @@
         <v>1185</v>
       </c>
       <c r="H14" s="164" t="s">
+        <v>1264</v>
+      </c>
+      <c r="I14" s="365" t="s">
         <v>1268</v>
       </c>
-      <c r="I14" s="365" t="s">
-        <v>1186</v>
-      </c>
       <c r="J14" s="357" t="s">
-        <v>1187</v>
+        <v>1267</v>
       </c>
       <c r="K14" s="357" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="N14" s="164" t="s">
         <v>1144</v>
       </c>
       <c r="O14" s="89" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="P14" s="89" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="Q14" s="89">
         <v>8</v>
@@ -48059,10 +48059,10 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="89" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="B15" s="89" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="F15" s="89" t="s">
         <v>1184</v>
@@ -48071,25 +48071,25 @@
         <v>1185</v>
       </c>
       <c r="H15" s="164" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="I15" s="365" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="J15" s="357" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="K15" s="357" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="N15" s="164" t="s">
         <v>1144</v>
       </c>
       <c r="O15" s="89" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="P15" s="89" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="Q15" s="89">
         <v>8</v>
@@ -48097,37 +48097,37 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="89" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="B16" s="89" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="F16" s="89" t="s">
         <v>1184</v>
       </c>
       <c r="G16" s="89" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="H16" s="164" t="s">
         <v>235</v>
       </c>
       <c r="I16" s="365" t="s">
-        <v>1195</v>
+        <v>1266</v>
       </c>
       <c r="J16" s="357" t="s">
-        <v>1196</v>
+        <v>1265</v>
       </c>
       <c r="K16" s="357" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="N16" s="164" t="s">
         <v>1144</v>
       </c>
       <c r="O16" s="89" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="P16" s="89" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="Q16" s="89">
         <v>8</v>
@@ -48138,10 +48138,10 @@
         <v>574</v>
       </c>
       <c r="B17" s="89" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="F17" s="89" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="G17" s="89" t="s">
         <v>571</v>
@@ -48153,69 +48153,69 @@
         <v>574</v>
       </c>
       <c r="J17" s="357" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="K17" s="357" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="N17" s="164" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="O17" s="89" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="P17" s="89" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="89" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="B18" s="89" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="F18" s="348"/>
       <c r="G18" s="349"/>
       <c r="H18" s="349"/>
       <c r="I18" s="53" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="J18" s="357" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="K18" s="357" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="L18" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M18" s="89" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="N18" s="351"/>
       <c r="O18" s="349"/>
       <c r="P18" s="349"/>
       <c r="Q18" s="349"/>
       <c r="R18" s="89" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="89" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="B19" s="89" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="F19" s="348"/>
       <c r="G19" s="349"/>
       <c r="H19" s="349"/>
       <c r="I19" s="89" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="J19" s="349" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="K19" s="349"/>
       <c r="N19" s="351"/>
@@ -48225,22 +48225,22 @@
     </row>
     <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="89" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="B20" s="89" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="F20" s="352" t="s">
         <v>1137</v>
       </c>
       <c r="G20" s="89" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="I20" s="89" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="J20" s="349" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="K20" s="349"/>
       <c r="N20" s="351"/>
@@ -48250,22 +48250,22 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="89" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="B21" s="89" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="F21" s="349"/>
       <c r="G21" s="349"/>
       <c r="H21" s="349"/>
       <c r="I21" s="89" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="J21" s="357" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="K21" s="357" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="L21" s="89" t="s">
         <v>38</v>
@@ -48278,40 +48278,40 @@
       <c r="P21" s="349"/>
       <c r="Q21" s="349"/>
       <c r="R21" s="89" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="89" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="B22" s="89" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="F22" s="349"/>
       <c r="G22" s="349"/>
       <c r="H22" s="349"/>
       <c r="I22" s="89" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="J22" s="357" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="K22" s="357" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="L22" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M22" s="89" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="N22" s="351"/>
       <c r="O22" s="349"/>
       <c r="P22" s="349"/>
       <c r="Q22" s="349"/>
       <c r="R22" s="89" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ny version med n-bin
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20393"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mw\git\ctd_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\temp\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE22018-1725-4E95-95E3-2818FD120F6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6713B59-4011-4368-BD07-5B180A885271}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3958" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3962" uniqueCount="1287">
   <si>
     <t>Model</t>
   </si>
@@ -4137,9 +4137,6 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>5351, 5355, 6378, 6384, 4361</t>
-  </si>
-  <si>
     <t>-5.0</t>
   </si>
   <si>
@@ -4492,6 +4489,21 @@
   </si>
   <si>
     <t>SIGMA_THETA_CTD</t>
+  </si>
+  <si>
+    <t>5351, 5355, 6378, 6384, 4361, 4387</t>
+  </si>
+  <si>
+    <t>SCAN_BIN_CTD</t>
+  </si>
+  <si>
+    <t>scans per bin</t>
+  </si>
+  <si>
+    <t>nbin</t>
+  </si>
+  <si>
+    <t>Number of scans per bin</t>
   </si>
 </sst>
 </file>
@@ -4691,7 +4703,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4743,18 +4755,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4989,7 +4989,7 @@
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="370">
+  <cellXfs count="366">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5894,16 +5894,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
@@ -5923,17 +5918,16 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Förklarande text 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -47524,18 +47518,18 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.875" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.625" style="89" customWidth="1"/>
+    <col min="2" max="2" width="23" style="89" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.375" style="89" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.125" style="89" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.875" style="89" bestFit="1" customWidth="1"/>
@@ -47555,7 +47549,7 @@
         <v>1099</v>
       </c>
       <c r="B1" s="345" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="C1" s="345" t="s">
         <v>390</v>
@@ -47582,7 +47576,7 @@
         <v>1106</v>
       </c>
       <c r="K1" s="345" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="L1" s="345" t="s">
         <v>1107</v>
@@ -47611,7 +47605,7 @@
         <v>1114</v>
       </c>
       <c r="B2" s="346" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="C2" s="346" t="s">
         <v>1115</v>
@@ -47638,7 +47632,7 @@
         <v>1122</v>
       </c>
       <c r="K2" s="346" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="L2" s="346" t="s">
         <v>1123</v>
@@ -47667,19 +47661,19 @@
         <v>1130</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>1257</v>
-      </c>
-      <c r="F3" s="348"/>
-      <c r="G3" s="349"/>
-      <c r="H3" s="349"/>
-      <c r="I3" s="350" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F3" s="362"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="349" t="s">
         <v>1131</v>
       </c>
-      <c r="J3" s="349" t="s">
+      <c r="J3" s="348" t="s">
         <v>1132</v>
       </c>
-      <c r="K3" s="349" t="s">
-        <v>1254</v>
+      <c r="K3" s="348" t="s">
+        <v>1253</v>
       </c>
       <c r="L3" s="89" t="s">
         <v>38</v>
@@ -47687,20 +47681,25 @@
       <c r="M3" s="89" t="s">
         <v>1133</v>
       </c>
-      <c r="N3" s="351"/>
-      <c r="O3" s="349"/>
-      <c r="P3" s="349"/>
-      <c r="Q3" s="349"/>
-      <c r="R3" s="89" t="s">
+      <c r="N3" s="359"/>
+      <c r="O3" s="183"/>
+      <c r="P3" s="183"/>
+      <c r="Q3" s="183"/>
+      <c r="R3" s="183" t="s">
         <v>1134</v>
       </c>
+      <c r="S3" s="183"/>
+      <c r="T3" s="183"/>
+      <c r="U3" s="183"/>
+      <c r="V3" s="183"/>
+      <c r="W3" s="183"/>
     </row>
     <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="89" t="s">
         <v>1135</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>1136</v>
@@ -47711,43 +47710,49 @@
       <c r="E4" s="89" t="s">
         <v>1138</v>
       </c>
-      <c r="F4" s="352" t="s">
+      <c r="F4" s="362" t="s">
         <v>1139</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="183" t="s">
         <v>1140</v>
       </c>
-      <c r="H4" s="164" t="s">
+      <c r="H4" s="359" t="s">
         <v>1141</v>
       </c>
-      <c r="I4" s="350" t="s">
+      <c r="I4" s="349" t="s">
         <v>1142</v>
       </c>
-      <c r="J4" s="349" t="s">
+      <c r="J4" s="348" t="s">
         <v>1143</v>
       </c>
-      <c r="K4" s="349" t="s">
-        <v>1244</v>
-      </c>
-      <c r="N4" s="164" t="s">
+      <c r="K4" s="348" t="s">
+        <v>1243</v>
+      </c>
+      <c r="N4" s="359" t="s">
         <v>1144</v>
       </c>
-      <c r="O4" s="89" t="s">
+      <c r="O4" s="183" t="s">
         <v>1145</v>
       </c>
-      <c r="P4" s="89" t="s">
+      <c r="P4" s="183" t="s">
         <v>1146</v>
       </c>
-      <c r="Q4" s="89">
+      <c r="Q4" s="183">
         <v>24</v>
       </c>
+      <c r="R4" s="183"/>
+      <c r="S4" s="183"/>
+      <c r="T4" s="183"/>
+      <c r="U4" s="183"/>
+      <c r="V4" s="183"/>
+      <c r="W4" s="183"/>
     </row>
     <row r="5" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="89" t="s">
         <v>1135</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>1136</v>
@@ -47758,138 +47763,152 @@
       <c r="E5" s="89" t="s">
         <v>1147</v>
       </c>
-      <c r="F5" s="352" t="s">
+      <c r="F5" s="362" t="s">
         <v>1137</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="G5" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H5" s="353">
+      <c r="H5" s="363">
         <v>6164</v>
       </c>
-      <c r="I5" s="350" t="s">
+      <c r="I5" s="349" t="s">
         <v>1142</v>
       </c>
-      <c r="J5" s="349" t="s">
+      <c r="J5" s="348" t="s">
         <v>1143</v>
       </c>
-      <c r="K5" s="349" t="s">
-        <v>1244</v>
-      </c>
-      <c r="N5" s="354"/>
-      <c r="O5" s="355" t="s">
+      <c r="K5" s="348" t="s">
+        <v>1243</v>
+      </c>
+      <c r="N5" s="351"/>
+      <c r="O5" s="352" t="s">
         <v>1149</v>
       </c>
-      <c r="P5" s="354" t="s">
+      <c r="P5" s="351" t="s">
         <v>1150</v>
       </c>
-      <c r="Q5" s="355">
+      <c r="Q5" s="352">
         <v>4</v>
       </c>
-      <c r="R5" s="356" t="s">
+      <c r="R5" s="353" t="s">
         <v>1151</v>
       </c>
+      <c r="S5" s="183"/>
+      <c r="T5" s="183"/>
+      <c r="U5" s="183"/>
+      <c r="V5" s="183"/>
+      <c r="W5" s="183"/>
     </row>
     <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="89" t="s">
         <v>1152</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>1235</v>
-      </c>
-      <c r="F6" s="352" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F6" s="362" t="s">
         <v>1137</v>
       </c>
-      <c r="G6" s="350" t="s">
+      <c r="G6" s="349" t="s">
         <v>199</v>
       </c>
-      <c r="H6" s="164" t="s">
+      <c r="H6" s="359" t="s">
         <v>1153</v>
       </c>
-      <c r="I6" s="350" t="s">
-        <v>1221</v>
-      </c>
-      <c r="J6" s="357" t="s">
-        <v>1216</v>
-      </c>
-      <c r="K6" s="357" t="s">
-        <v>1245</v>
-      </c>
-      <c r="L6" s="358"/>
-      <c r="M6" s="358"/>
-      <c r="N6" s="164" t="s">
+      <c r="I6" s="349" t="s">
+        <v>1220</v>
+      </c>
+      <c r="J6" s="354" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K6" s="354" t="s">
+        <v>1244</v>
+      </c>
+      <c r="L6" s="355"/>
+      <c r="M6" s="355"/>
+      <c r="N6" s="359" t="s">
         <v>1144</v>
       </c>
-      <c r="O6" s="89" t="s">
+      <c r="O6" s="183" t="s">
         <v>1154</v>
       </c>
-      <c r="P6" s="89" t="s">
+      <c r="P6" s="183" t="s">
         <v>1155</v>
       </c>
-      <c r="Q6" s="89">
+      <c r="Q6" s="183">
         <v>24</v>
       </c>
+      <c r="R6" s="183"/>
+      <c r="S6" s="183"/>
+      <c r="T6" s="183"/>
+      <c r="U6" s="183"/>
+      <c r="V6" s="183"/>
+      <c r="W6" s="183"/>
     </row>
     <row r="7" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
         <v>1152</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>1235</v>
-      </c>
-      <c r="F7" s="352" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F7" s="362" t="s">
         <v>1137</v>
       </c>
-      <c r="G7" s="89" t="s">
+      <c r="G7" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H7" s="353">
+      <c r="H7" s="363">
         <v>6164</v>
       </c>
-      <c r="I7" s="350" t="s">
-        <v>1221</v>
-      </c>
-      <c r="J7" s="357" t="s">
-        <v>1216</v>
-      </c>
-      <c r="K7" s="357" t="s">
-        <v>1245</v>
-      </c>
-      <c r="L7" s="359"/>
-      <c r="O7" s="359" t="s">
+      <c r="I7" s="349" t="s">
+        <v>1220</v>
+      </c>
+      <c r="J7" s="354" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K7" s="354" t="s">
+        <v>1244</v>
+      </c>
+      <c r="L7" s="356"/>
+      <c r="N7" s="183"/>
+      <c r="O7" s="356" t="s">
         <v>1156</v>
       </c>
-      <c r="P7" s="359" t="s">
+      <c r="P7" s="356" t="s">
         <v>1157</v>
       </c>
-      <c r="Q7" s="360">
+      <c r="Q7" s="357">
         <v>4</v>
       </c>
       <c r="R7" s="183" t="s">
         <v>1158</v>
       </c>
-      <c r="U7" s="350"/>
-      <c r="V7" s="357"/>
-      <c r="W7" s="361"/>
+      <c r="S7" s="183"/>
+      <c r="T7" s="183"/>
+      <c r="U7" s="349"/>
+      <c r="V7" s="349"/>
+      <c r="W7" s="358"/>
     </row>
     <row r="8" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="89" t="s">
         <v>1159</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>1236</v>
-      </c>
-      <c r="F8" s="348"/>
-      <c r="G8" s="349"/>
-      <c r="H8" s="351"/>
-      <c r="I8" s="350" t="s">
-        <v>1222</v>
-      </c>
-      <c r="J8" s="349" t="s">
-        <v>1217</v>
-      </c>
-      <c r="K8" s="349" t="s">
-        <v>1246</v>
+        <v>1235</v>
+      </c>
+      <c r="F8" s="362"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="359"/>
+      <c r="I8" s="349" t="s">
+        <v>1221</v>
+      </c>
+      <c r="J8" s="348" t="s">
+        <v>1216</v>
+      </c>
+      <c r="K8" s="348" t="s">
+        <v>1245</v>
       </c>
       <c r="L8" s="89" t="s">
         <v>38</v>
@@ -47897,476 +47916,554 @@
       <c r="M8" s="89" t="s">
         <v>1160</v>
       </c>
-      <c r="N8" s="362" t="s">
+      <c r="N8" s="359" t="s">
         <v>1161</v>
       </c>
-      <c r="O8" s="363"/>
-      <c r="P8" s="363"/>
-      <c r="Q8" s="363"/>
-      <c r="R8" s="89" t="s">
+      <c r="O8" s="364"/>
+      <c r="P8" s="364"/>
+      <c r="Q8" s="364"/>
+      <c r="R8" s="183" t="s">
         <v>1162</v>
       </c>
+      <c r="S8" s="183"/>
+      <c r="T8" s="183"/>
+      <c r="U8" s="183"/>
+      <c r="V8" s="183"/>
+      <c r="W8" s="183"/>
     </row>
     <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
         <v>1163</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>1232</v>
-      </c>
-      <c r="F9" s="352" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F9" s="362" t="s">
         <v>1137</v>
       </c>
-      <c r="G9" s="352" t="s">
+      <c r="G9" s="362" t="s">
         <v>647</v>
       </c>
-      <c r="H9" s="164" t="s">
+      <c r="H9" s="359" t="s">
+        <v>1282</v>
+      </c>
+      <c r="I9" s="349" t="s">
+        <v>1222</v>
+      </c>
+      <c r="J9" s="348" t="s">
+        <v>1217</v>
+      </c>
+      <c r="K9" s="348" t="s">
+        <v>1246</v>
+      </c>
+      <c r="L9" s="350"/>
+      <c r="M9" s="350"/>
+      <c r="N9" s="359" t="s">
         <v>1164</v>
       </c>
-      <c r="I9" s="350" t="s">
-        <v>1223</v>
-      </c>
-      <c r="J9" s="349" t="s">
-        <v>1218</v>
-      </c>
-      <c r="K9" s="349" t="s">
-        <v>1247</v>
-      </c>
-      <c r="L9" s="352"/>
-      <c r="M9" s="352"/>
-      <c r="N9" s="164" t="s">
+      <c r="O9" s="365" t="s">
         <v>1165</v>
       </c>
-      <c r="O9" s="364" t="s">
+      <c r="P9" s="183" t="s">
         <v>1166</v>
       </c>
-      <c r="P9" s="89" t="s">
-        <v>1167</v>
-      </c>
-      <c r="Q9" s="89">
+      <c r="Q9" s="183">
         <v>24</v>
       </c>
+      <c r="R9" s="183"/>
+      <c r="S9" s="183"/>
+      <c r="T9" s="183"/>
+      <c r="U9" s="183"/>
+      <c r="V9" s="183"/>
+      <c r="W9" s="183"/>
     </row>
     <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="89" t="s">
         <v>1163</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>1232</v>
-      </c>
-      <c r="F10" s="352" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F10" s="362" t="s">
         <v>1137</v>
       </c>
-      <c r="G10" s="89" t="s">
+      <c r="G10" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H10" s="353">
+      <c r="H10" s="363">
         <v>6164</v>
       </c>
-      <c r="I10" s="350" t="s">
-        <v>1223</v>
-      </c>
-      <c r="J10" s="349" t="s">
-        <v>1218</v>
-      </c>
-      <c r="K10" s="349" t="s">
-        <v>1247</v>
-      </c>
-      <c r="L10" s="352"/>
-      <c r="M10" s="359"/>
-      <c r="O10" s="359" t="s">
+      <c r="I10" s="349" t="s">
+        <v>1222</v>
+      </c>
+      <c r="J10" s="348" t="s">
+        <v>1217</v>
+      </c>
+      <c r="K10" s="348" t="s">
+        <v>1246</v>
+      </c>
+      <c r="L10" s="350"/>
+      <c r="M10" s="356"/>
+      <c r="N10" s="183"/>
+      <c r="O10" s="356" t="s">
+        <v>1167</v>
+      </c>
+      <c r="P10" s="356" t="s">
         <v>1168</v>
       </c>
-      <c r="P10" s="359" t="s">
+      <c r="Q10" s="357">
+        <v>4</v>
+      </c>
+      <c r="R10" s="183" t="s">
         <v>1169</v>
       </c>
-      <c r="Q10" s="360">
-        <v>4</v>
-      </c>
-      <c r="R10" s="183" t="s">
-        <v>1170</v>
-      </c>
+      <c r="S10" s="183"/>
+      <c r="T10" s="183"/>
+      <c r="U10" s="183"/>
+      <c r="V10" s="183"/>
+      <c r="W10" s="183"/>
     </row>
     <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>1233</v>
-      </c>
-      <c r="F11" s="352" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F11" s="362" t="s">
         <v>1137</v>
       </c>
-      <c r="G11" s="352" t="s">
+      <c r="G11" s="362" t="s">
         <v>174</v>
       </c>
-      <c r="H11" s="164" t="s">
+      <c r="H11" s="359" t="s">
+        <v>1170</v>
+      </c>
+      <c r="I11" s="349" t="s">
+        <v>1223</v>
+      </c>
+      <c r="J11" s="348" t="s">
+        <v>1218</v>
+      </c>
+      <c r="K11" s="348" t="s">
+        <v>1247</v>
+      </c>
+      <c r="L11" s="350"/>
+      <c r="M11" s="350"/>
+      <c r="N11" s="359" t="s">
         <v>1171</v>
       </c>
-      <c r="I11" s="350" t="s">
+      <c r="O11" s="183" t="s">
+        <v>1172</v>
+      </c>
+      <c r="P11" s="183" t="s">
+        <v>566</v>
+      </c>
+      <c r="Q11" s="183" t="s">
+        <v>1173</v>
+      </c>
+      <c r="R11" s="183" t="s">
+        <v>1174</v>
+      </c>
+      <c r="S11" s="183"/>
+      <c r="T11" s="183"/>
+      <c r="U11" s="183"/>
+      <c r="V11" s="183"/>
+      <c r="W11" s="183"/>
+    </row>
+    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="183" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B12" s="183" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F12" s="362"/>
+      <c r="G12" s="183"/>
+      <c r="H12" s="359"/>
+      <c r="I12" s="349" t="s">
         <v>1224</v>
       </c>
-      <c r="J11" s="349" t="s">
-        <v>1219</v>
-      </c>
-      <c r="K11" s="349" t="s">
-        <v>1248</v>
-      </c>
-      <c r="L11" s="352"/>
-      <c r="M11" s="352"/>
-      <c r="N11" s="164" t="s">
-        <v>1172</v>
-      </c>
-      <c r="O11" s="89" t="s">
-        <v>1173</v>
-      </c>
-      <c r="P11" s="89" t="s">
-        <v>566</v>
-      </c>
-      <c r="Q11" s="89" t="s">
-        <v>1174</v>
-      </c>
-      <c r="R11" s="89" t="s">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B12" s="366" t="s">
-        <v>1268</v>
-      </c>
-      <c r="F12" s="348"/>
-      <c r="G12" s="349"/>
-      <c r="H12" s="351"/>
-      <c r="I12" s="350" t="s">
-        <v>1225</v>
-      </c>
-      <c r="J12" s="368" t="s">
-        <v>1278</v>
-      </c>
-      <c r="K12" s="349" t="s">
-        <v>1250</v>
+      <c r="J12" s="348" t="s">
+        <v>1277</v>
+      </c>
+      <c r="K12" s="348" t="s">
+        <v>1249</v>
       </c>
       <c r="L12" s="89" t="s">
         <v>38</v>
       </c>
+      <c r="N12" s="183"/>
+      <c r="O12" s="183"/>
+      <c r="P12" s="183"/>
+      <c r="Q12" s="183"/>
+      <c r="R12" s="183"/>
+      <c r="S12" s="183"/>
+      <c r="T12" s="183"/>
+      <c r="U12" s="183"/>
+      <c r="V12" s="183"/>
+      <c r="W12" s="183"/>
     </row>
     <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="183" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B13" s="183" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F13" s="362" t="s">
         <v>1177</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="G13" s="362" t="s">
+        <v>1178</v>
+      </c>
+      <c r="H13" s="359" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I13" s="89" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J13" s="348" t="s">
+        <v>1180</v>
+      </c>
+      <c r="K13" s="348" t="s">
+        <v>1248</v>
+      </c>
+      <c r="L13" s="350"/>
+      <c r="M13" s="350"/>
+      <c r="N13" s="359" t="s">
+        <v>1181</v>
+      </c>
+      <c r="O13" s="183" t="s">
+        <v>1182</v>
+      </c>
+      <c r="P13" s="183"/>
+      <c r="Q13" s="183"/>
+      <c r="R13" s="183"/>
+      <c r="S13" s="183"/>
+      <c r="T13" s="183"/>
+      <c r="U13" s="183"/>
+      <c r="V13" s="183"/>
+      <c r="W13" s="183"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="183" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B14" s="183" t="s">
         <v>1237</v>
       </c>
-      <c r="F13" s="352" t="s">
-        <v>1178</v>
-      </c>
-      <c r="G13" s="352" t="s">
-        <v>1179</v>
-      </c>
-      <c r="H13" s="164" t="s">
+      <c r="F14" s="183" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G14" s="183" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H14" s="359" t="s">
+        <v>1274</v>
+      </c>
+      <c r="I14" s="53" t="s">
+        <v>1264</v>
+      </c>
+      <c r="J14" s="354" t="s">
+        <v>1263</v>
+      </c>
+      <c r="K14" s="354" t="s">
+        <v>1250</v>
+      </c>
+      <c r="N14" s="359" t="s">
+        <v>1144</v>
+      </c>
+      <c r="O14" s="183" t="s">
+        <v>1185</v>
+      </c>
+      <c r="P14" s="183" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Q14" s="183">
+        <v>8</v>
+      </c>
+      <c r="R14" s="183"/>
+      <c r="S14" s="183"/>
+      <c r="T14" s="183"/>
+      <c r="U14" s="183"/>
+      <c r="V14" s="183"/>
+      <c r="W14" s="183"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="183" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B15" s="183" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F15" s="183" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G15" s="183" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H15" s="359" t="s">
+        <v>1274</v>
+      </c>
+      <c r="I15" s="53" t="s">
+        <v>1187</v>
+      </c>
+      <c r="J15" s="354" t="s">
+        <v>1188</v>
+      </c>
+      <c r="K15" s="354" t="s">
+        <v>1251</v>
+      </c>
+      <c r="N15" s="359" t="s">
+        <v>1144</v>
+      </c>
+      <c r="O15" s="183" t="s">
+        <v>1189</v>
+      </c>
+      <c r="P15" s="183" t="s">
+        <v>1190</v>
+      </c>
+      <c r="Q15" s="183">
+        <v>8</v>
+      </c>
+      <c r="R15" s="183"/>
+      <c r="S15" s="183"/>
+      <c r="T15" s="183"/>
+      <c r="U15" s="183"/>
+      <c r="V15" s="183"/>
+      <c r="W15" s="183"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="183" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B16" s="183" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F16" s="183" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G16" s="183" t="s">
+        <v>1191</v>
+      </c>
+      <c r="H16" s="359" t="s">
+        <v>235</v>
+      </c>
+      <c r="I16" s="53" t="s">
+        <v>1262</v>
+      </c>
+      <c r="J16" s="354" t="s">
+        <v>1261</v>
+      </c>
+      <c r="K16" s="354" t="s">
+        <v>1252</v>
+      </c>
+      <c r="N16" s="359" t="s">
+        <v>1144</v>
+      </c>
+      <c r="O16" s="183" t="s">
+        <v>1192</v>
+      </c>
+      <c r="P16" s="183" t="s">
+        <v>1193</v>
+      </c>
+      <c r="Q16" s="183">
+        <v>8</v>
+      </c>
+      <c r="R16" s="183"/>
+      <c r="S16" s="183"/>
+      <c r="T16" s="183"/>
+      <c r="U16" s="183"/>
+      <c r="V16" s="183"/>
+      <c r="W16" s="183"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="183" t="s">
+        <v>574</v>
+      </c>
+      <c r="B17" s="183" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F17" s="183" t="s">
+        <v>1194</v>
+      </c>
+      <c r="G17" s="183" t="s">
+        <v>571</v>
+      </c>
+      <c r="H17" s="359" t="s">
         <v>1266</v>
-      </c>
-      <c r="I13" s="89" t="s">
-        <v>1180</v>
-      </c>
-      <c r="J13" s="349" t="s">
-        <v>1181</v>
-      </c>
-      <c r="K13" s="349" t="s">
-        <v>1249</v>
-      </c>
-      <c r="L13" s="352"/>
-      <c r="M13" s="352"/>
-      <c r="N13" s="164" t="s">
-        <v>1182</v>
-      </c>
-      <c r="O13" s="89" t="s">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="89" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B14" s="89" t="s">
-        <v>1238</v>
-      </c>
-      <c r="F14" s="89" t="s">
-        <v>1184</v>
-      </c>
-      <c r="G14" s="89" t="s">
-        <v>1185</v>
-      </c>
-      <c r="H14" s="164" t="s">
-        <v>1275</v>
-      </c>
-      <c r="I14" s="365" t="s">
-        <v>1265</v>
-      </c>
-      <c r="J14" s="357" t="s">
-        <v>1264</v>
-      </c>
-      <c r="K14" s="357" t="s">
-        <v>1251</v>
-      </c>
-      <c r="N14" s="164" t="s">
-        <v>1144</v>
-      </c>
-      <c r="O14" s="89" t="s">
-        <v>1186</v>
-      </c>
-      <c r="P14" s="89" t="s">
-        <v>1187</v>
-      </c>
-      <c r="Q14" s="89">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="89" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B15" s="89" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F15" s="89" t="s">
-        <v>1184</v>
-      </c>
-      <c r="G15" s="89" t="s">
-        <v>1185</v>
-      </c>
-      <c r="H15" s="164" t="s">
-        <v>1275</v>
-      </c>
-      <c r="I15" s="365" t="s">
-        <v>1188</v>
-      </c>
-      <c r="J15" s="357" t="s">
-        <v>1189</v>
-      </c>
-      <c r="K15" s="357" t="s">
-        <v>1252</v>
-      </c>
-      <c r="N15" s="164" t="s">
-        <v>1144</v>
-      </c>
-      <c r="O15" s="89" t="s">
-        <v>1190</v>
-      </c>
-      <c r="P15" s="89" t="s">
-        <v>1191</v>
-      </c>
-      <c r="Q15" s="89">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="89" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B16" s="89" t="s">
-        <v>1238</v>
-      </c>
-      <c r="F16" s="89" t="s">
-        <v>1184</v>
-      </c>
-      <c r="G16" s="89" t="s">
-        <v>1192</v>
-      </c>
-      <c r="H16" s="164" t="s">
-        <v>235</v>
-      </c>
-      <c r="I16" s="365" t="s">
-        <v>1263</v>
-      </c>
-      <c r="J16" s="357" t="s">
-        <v>1262</v>
-      </c>
-      <c r="K16" s="357" t="s">
-        <v>1253</v>
-      </c>
-      <c r="N16" s="164" t="s">
-        <v>1144</v>
-      </c>
-      <c r="O16" s="89" t="s">
-        <v>1193</v>
-      </c>
-      <c r="P16" s="89" t="s">
-        <v>1194</v>
-      </c>
-      <c r="Q16" s="89">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="89" t="s">
-        <v>574</v>
-      </c>
-      <c r="B17" s="89" t="s">
-        <v>1240</v>
-      </c>
-      <c r="F17" s="89" t="s">
-        <v>1195</v>
-      </c>
-      <c r="G17" s="89" t="s">
-        <v>571</v>
-      </c>
-      <c r="H17" s="164" t="s">
-        <v>1267</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>574</v>
       </c>
-      <c r="J17" s="357" t="s">
+      <c r="J17" s="354" t="s">
+        <v>1195</v>
+      </c>
+      <c r="K17" s="354" t="s">
+        <v>1253</v>
+      </c>
+      <c r="N17" s="359" t="s">
         <v>1196</v>
       </c>
-      <c r="K17" s="357" t="s">
+      <c r="O17" s="183" t="s">
+        <v>1197</v>
+      </c>
+      <c r="P17" s="183" t="s">
+        <v>1198</v>
+      </c>
+      <c r="Q17" s="183"/>
+      <c r="R17" s="183"/>
+      <c r="S17" s="183"/>
+      <c r="T17" s="183"/>
+      <c r="U17" s="183"/>
+      <c r="V17" s="183"/>
+      <c r="W17" s="183"/>
+    </row>
+    <row r="18" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="183" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B18" s="183" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F18" s="362"/>
+      <c r="G18" s="183"/>
+      <c r="H18" s="183"/>
+      <c r="I18" s="53" t="s">
+        <v>1200</v>
+      </c>
+      <c r="J18" s="354" t="s">
+        <v>1201</v>
+      </c>
+      <c r="K18" s="354" t="s">
         <v>1254</v>
-      </c>
-      <c r="N17" s="164" t="s">
-        <v>1197</v>
-      </c>
-      <c r="O17" s="89" t="s">
-        <v>1198</v>
-      </c>
-      <c r="P17" s="89" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="89" t="s">
-        <v>1200</v>
-      </c>
-      <c r="B18" s="89" t="s">
-        <v>1260</v>
-      </c>
-      <c r="F18" s="348"/>
-      <c r="G18" s="349"/>
-      <c r="H18" s="349"/>
-      <c r="I18" s="53" t="s">
-        <v>1201</v>
-      </c>
-      <c r="J18" s="357" t="s">
-        <v>1202</v>
-      </c>
-      <c r="K18" s="357" t="s">
-        <v>1255</v>
       </c>
       <c r="L18" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M18" s="89" t="s">
+        <v>1202</v>
+      </c>
+      <c r="N18" s="359"/>
+      <c r="O18" s="183"/>
+      <c r="P18" s="183"/>
+      <c r="Q18" s="183"/>
+      <c r="R18" s="183" t="s">
         <v>1203</v>
       </c>
-      <c r="N18" s="351"/>
-      <c r="O18" s="349"/>
-      <c r="P18" s="349"/>
-      <c r="Q18" s="349"/>
-      <c r="R18" s="89" t="s">
+      <c r="S18" s="183"/>
+      <c r="T18" s="183"/>
+      <c r="U18" s="183"/>
+      <c r="V18" s="183"/>
+      <c r="W18" s="183"/>
+    </row>
+    <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="183" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B19" s="183" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F19" s="362"/>
+      <c r="G19" s="183"/>
+      <c r="H19" s="183"/>
+      <c r="I19" s="53" t="s">
+        <v>1284</v>
+      </c>
+      <c r="J19" s="354" t="s">
+        <v>1283</v>
+      </c>
+      <c r="K19" s="354"/>
+      <c r="N19" s="359"/>
+      <c r="O19" s="183"/>
+      <c r="P19" s="183"/>
+      <c r="Q19" s="183"/>
+      <c r="R19" s="183"/>
+      <c r="S19" s="183"/>
+      <c r="T19" s="183"/>
+      <c r="U19" s="183"/>
+      <c r="V19" s="183"/>
+      <c r="W19" s="183"/>
+    </row>
+    <row r="20" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="183" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="89" t="s">
+      <c r="B20" s="183" t="s">
+        <v>1258</v>
+      </c>
+      <c r="F20" s="362"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="89" t="s">
         <v>1205</v>
       </c>
-      <c r="B19" s="89" t="s">
-        <v>1259</v>
-      </c>
-      <c r="F19" s="348"/>
-      <c r="G19" s="349"/>
-      <c r="H19" s="349"/>
-      <c r="I19" s="89" t="s">
+      <c r="J20" s="348" t="s">
         <v>1206</v>
       </c>
-      <c r="J19" s="349" t="s">
+      <c r="K20" s="348"/>
+      <c r="N20" s="359"/>
+      <c r="O20" s="183"/>
+      <c r="P20" s="183"/>
+      <c r="Q20" s="183"/>
+      <c r="R20" s="183"/>
+      <c r="S20" s="183"/>
+      <c r="T20" s="183"/>
+      <c r="U20" s="183"/>
+      <c r="V20" s="183"/>
+      <c r="W20" s="183"/>
+    </row>
+    <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="183" t="s">
         <v>1207</v>
       </c>
-      <c r="K19" s="349"/>
-      <c r="N19" s="351"/>
-      <c r="O19" s="349"/>
-      <c r="P19" s="349"/>
-      <c r="Q19" s="349"/>
-    </row>
-    <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="89" t="s">
+      <c r="B21" s="183" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F21" s="362" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G21" s="183" t="s">
         <v>1208</v>
       </c>
-      <c r="B20" s="89" t="s">
-        <v>1261</v>
-      </c>
-      <c r="F20" s="352" t="s">
-        <v>1137</v>
-      </c>
-      <c r="G20" s="89" t="s">
+      <c r="H21" s="183"/>
+      <c r="I21" s="89" t="s">
         <v>1209</v>
       </c>
-      <c r="I20" s="89" t="s">
+      <c r="J21" s="348" t="s">
         <v>1210</v>
       </c>
-      <c r="J20" s="349" t="s">
+      <c r="K21" s="348"/>
+      <c r="N21" s="359"/>
+      <c r="O21" s="359"/>
+      <c r="P21" s="359"/>
+      <c r="Q21" s="359"/>
+      <c r="R21" s="183"/>
+      <c r="S21" s="183"/>
+      <c r="T21" s="183"/>
+      <c r="U21" s="183"/>
+      <c r="V21" s="183"/>
+      <c r="W21" s="183"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" s="183" t="s">
         <v>1211</v>
       </c>
-      <c r="K20" s="349"/>
-      <c r="N20" s="351"/>
-      <c r="O20" s="351"/>
-      <c r="P20" s="351"/>
-      <c r="Q20" s="351"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="89" t="s">
-        <v>1212</v>
-      </c>
-      <c r="B21" s="89" t="s">
+      <c r="B22" s="183" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F22" s="183"/>
+      <c r="G22" s="183"/>
+      <c r="H22" s="183"/>
+      <c r="I22" s="89" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J22" s="354" t="s">
         <v>1281</v>
       </c>
-      <c r="F21" s="349"/>
-      <c r="G21" s="349"/>
-      <c r="H21" s="349"/>
-      <c r="I21" s="89" t="s">
-        <v>1226</v>
-      </c>
-      <c r="J21" s="357" t="s">
-        <v>1282</v>
-      </c>
-      <c r="K21" s="357" t="s">
-        <v>1256</v>
-      </c>
-      <c r="L21" s="89" t="s">
-        <v>38</v>
-      </c>
-      <c r="M21" s="89" t="s">
-        <v>1160</v>
-      </c>
-      <c r="N21" s="351"/>
-      <c r="O21" s="349"/>
-      <c r="P21" s="349"/>
-      <c r="Q21" s="349"/>
-      <c r="R21" s="89" t="s">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="89" t="s">
-        <v>1212</v>
-      </c>
-      <c r="B22" s="89" t="s">
-        <v>1276</v>
-      </c>
-      <c r="F22" s="349"/>
-      <c r="G22" s="349"/>
-      <c r="H22" s="349"/>
-      <c r="I22" s="89" t="s">
-        <v>1226</v>
-      </c>
-      <c r="J22" s="357" t="s">
-        <v>1277</v>
-      </c>
-      <c r="K22" s="357" t="s">
-        <v>1256</v>
+      <c r="K22" s="354" t="s">
+        <v>1255</v>
       </c>
       <c r="L22" s="89" t="s">
         <v>38</v>
@@ -48374,86 +48471,154 @@
       <c r="M22" s="89" t="s">
         <v>1160</v>
       </c>
-      <c r="N22" s="351"/>
-      <c r="O22" s="349"/>
-      <c r="P22" s="349"/>
-      <c r="Q22" s="349"/>
-      <c r="R22" s="89" t="s">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="89" t="s">
-        <v>1214</v>
-      </c>
-      <c r="B23" s="89" t="s">
-        <v>1258</v>
-      </c>
-      <c r="F23" s="349"/>
-      <c r="G23" s="349"/>
-      <c r="H23" s="349"/>
+      <c r="N22" s="359"/>
+      <c r="O22" s="183"/>
+      <c r="P22" s="183"/>
+      <c r="Q22" s="183"/>
+      <c r="R22" s="183" t="s">
+        <v>1212</v>
+      </c>
+      <c r="S22" s="183"/>
+      <c r="T22" s="183"/>
+      <c r="U22" s="183"/>
+      <c r="V22" s="183"/>
+      <c r="W22" s="183"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="183" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B23" s="183" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F23" s="183"/>
+      <c r="G23" s="183"/>
+      <c r="H23" s="183"/>
       <c r="I23" s="89" t="s">
-        <v>1227</v>
-      </c>
-      <c r="J23" s="357" t="s">
-        <v>1220</v>
-      </c>
-      <c r="K23" s="357" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J23" s="354" t="s">
+        <v>1276</v>
+      </c>
+      <c r="K23" s="354" t="s">
         <v>1255</v>
       </c>
       <c r="L23" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M23" s="89" t="s">
-        <v>1215</v>
-      </c>
-      <c r="N23" s="351"/>
-      <c r="O23" s="349"/>
-      <c r="P23" s="349"/>
-      <c r="Q23" s="349"/>
-      <c r="R23" s="89" t="s">
+        <v>1160</v>
+      </c>
+      <c r="N23" s="359"/>
+      <c r="O23" s="183"/>
+      <c r="P23" s="183"/>
+      <c r="Q23" s="183"/>
+      <c r="R23" s="183" t="s">
+        <v>1212</v>
+      </c>
+      <c r="S23" s="183"/>
+      <c r="T23" s="183"/>
+      <c r="U23" s="183"/>
+      <c r="V23" s="183"/>
+      <c r="W23" s="183"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" s="183" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="366" t="s">
+      <c r="B24" s="183" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F24" s="183"/>
+      <c r="G24" s="183"/>
+      <c r="H24" s="183"/>
+      <c r="I24" s="89" t="s">
+        <v>1226</v>
+      </c>
+      <c r="J24" s="354" t="s">
+        <v>1219</v>
+      </c>
+      <c r="K24" s="354" t="s">
+        <v>1254</v>
+      </c>
+      <c r="L24" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="M24" s="89" t="s">
+        <v>1214</v>
+      </c>
+      <c r="N24" s="359"/>
+      <c r="O24" s="183"/>
+      <c r="P24" s="183"/>
+      <c r="Q24" s="183"/>
+      <c r="R24" s="183" t="s">
+        <v>1212</v>
+      </c>
+      <c r="S24" s="183"/>
+      <c r="T24" s="183"/>
+      <c r="U24" s="183"/>
+      <c r="V24" s="183"/>
+      <c r="W24" s="183"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" s="183" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B25" s="183" t="s">
         <v>1269</v>
       </c>
-      <c r="B24" s="366" t="s">
+      <c r="F25" s="183"/>
+      <c r="G25" s="183"/>
+      <c r="H25" s="183"/>
+      <c r="I25" s="360" t="s">
         <v>1270</v>
       </c>
-      <c r="I24" s="367" t="s">
+      <c r="J25" s="354" t="s">
+        <v>1278</v>
+      </c>
+      <c r="K25" s="354" t="s">
+        <v>1245</v>
+      </c>
+      <c r="L25" s="360" t="s">
+        <v>38</v>
+      </c>
+      <c r="N25" s="183"/>
+      <c r="O25" s="183"/>
+      <c r="P25" s="183"/>
+      <c r="Q25" s="183"/>
+      <c r="R25" s="183"/>
+      <c r="S25" s="183"/>
+      <c r="T25" s="183"/>
+      <c r="U25" s="183"/>
+      <c r="V25" s="183"/>
+      <c r="W25" s="183"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" s="183" t="s">
         <v>1271</v>
       </c>
-      <c r="J24" s="369" t="s">
+      <c r="B26" s="183" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F26" s="183"/>
+      <c r="G26" s="183"/>
+      <c r="H26" s="183"/>
+      <c r="I26" s="361" t="s">
+        <v>1273</v>
+      </c>
+      <c r="J26" s="348" t="s">
         <v>1279</v>
       </c>
-      <c r="K24" s="367" t="s">
+      <c r="K26" s="348" t="s">
         <v>1246</v>
       </c>
-      <c r="L24" s="367" t="s">
+      <c r="L26" s="361" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="366" t="s">
-        <v>1272</v>
-      </c>
-      <c r="B25" s="366" t="s">
-        <v>1273</v>
-      </c>
-      <c r="I25" s="366" t="s">
-        <v>1274</v>
-      </c>
-      <c r="J25" s="368" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K25" s="366" t="s">
-        <v>1247</v>
-      </c>
-      <c r="L25" s="366" t="s">
-        <v>38</v>
-      </c>
+      <c r="N26" s="183"/>
+      <c r="O26" s="183"/>
+      <c r="P26" s="183"/>
+      <c r="Q26" s="183"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated altimeter 1251 serieno
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20393"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\temp\ctd_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6713B59-4011-4368-BD07-5B180A885271}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="SBE MicroCATs" sheetId="1" r:id="rId1"/>
@@ -58,12 +57,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,12 +91,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>ocean.gbg11</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000002000000}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000003000000}">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000004000000}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -204,12 +203,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -238,12 +237,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,12 +271,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1000-000001000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4443,9 +4442,6 @@
     <t>70374, 70711</t>
   </si>
   <si>
-    <t>53447, 71991</t>
-  </si>
-  <si>
     <t>sbeox0PS, sbeox1PS</t>
   </si>
   <si>
@@ -4504,12 +4500,15 @@
   </si>
   <si>
     <t>Number of scans per bin</t>
+  </si>
+  <si>
+    <t>53447, 71991, 1251</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
@@ -5930,12 +5929,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Förklarande text 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlänk 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Förklarande text 2" xfId="4"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlänk 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="1602">
     <dxf>
@@ -17644,7 +17643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -23666,79 +23665,79 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>W26:W1048576 W1:W17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576 W18:W25</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$23</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$M:$M</xm:f>
           </x14:formula1>
@@ -23751,7 +23750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -24705,25 +24704,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -24736,7 +24735,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -25586,25 +25585,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -25617,7 +25616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -27212,19 +27211,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$45</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -27237,7 +27236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -29112,31 +29111,31 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$3:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$N$2:$N$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
@@ -29149,7 +29148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -29161,7 +29160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -33175,73 +33174,73 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0E00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>AA1:AA1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0E00-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
           <xm:sqref>Z1:Z1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej" xr:uid="{00000000-0002-0000-0E00-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej">
           <x14:formula1>
             <xm:f>Listor!$M$3:$M$7</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A:$A</xm:f>
           </x14:formula1>
@@ -33254,7 +33253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -45068,19 +45067,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -45093,7 +45092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -46921,19 +46920,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -46946,7 +46945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -47517,13 +47516,13 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H22:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -47945,7 +47944,7 @@
         <v>647</v>
       </c>
       <c r="H9" s="359" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I9" s="349" t="s">
         <v>1222</v>
@@ -48076,7 +48075,7 @@
         <v>1175</v>
       </c>
       <c r="B12" s="183" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="F12" s="362"/>
       <c r="G12" s="183"/>
@@ -48085,7 +48084,7 @@
         <v>1224</v>
       </c>
       <c r="J12" s="348" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="K12" s="348" t="s">
         <v>1249</v>
@@ -48160,7 +48159,7 @@
         <v>1184</v>
       </c>
       <c r="H14" s="359" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="I14" s="53" t="s">
         <v>1264</v>
@@ -48204,7 +48203,7 @@
         <v>1184</v>
       </c>
       <c r="H15" s="359" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>1187</v>
@@ -48292,7 +48291,7 @@
         <v>571</v>
       </c>
       <c r="H17" s="359" t="s">
-        <v>1266</v>
+        <v>1286</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>574</v>
@@ -48360,19 +48359,19 @@
     </row>
     <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="183" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B19" s="183" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="F19" s="362"/>
       <c r="G19" s="183"/>
       <c r="H19" s="183"/>
       <c r="I19" s="53" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="J19" s="354" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="K19" s="354"/>
       <c r="N19" s="359"/>
@@ -48451,7 +48450,7 @@
         <v>1211</v>
       </c>
       <c r="B22" s="183" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="F22" s="183"/>
       <c r="G22" s="183"/>
@@ -48460,7 +48459,7 @@
         <v>1225</v>
       </c>
       <c r="J22" s="354" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="K22" s="354" t="s">
         <v>1255</v>
@@ -48489,7 +48488,7 @@
         <v>1211</v>
       </c>
       <c r="B23" s="183" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
@@ -48498,7 +48497,7 @@
         <v>1225</v>
       </c>
       <c r="J23" s="354" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="K23" s="354" t="s">
         <v>1255</v>
@@ -48562,19 +48561,19 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="183" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B25" s="183" t="s">
         <v>1268</v>
-      </c>
-      <c r="B25" s="183" t="s">
-        <v>1269</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
       <c r="H25" s="183"/>
       <c r="I25" s="360" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="J25" s="354" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="K25" s="354" t="s">
         <v>1245</v>
@@ -48595,19 +48594,19 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="183" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B26" s="183" t="s">
         <v>1271</v>
-      </c>
-      <c r="B26" s="183" t="s">
-        <v>1272</v>
       </c>
       <c r="F26" s="183"/>
       <c r="G26" s="183"/>
       <c r="H26" s="183"/>
       <c r="I26" s="361" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="J26" s="348" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="K26" s="348" t="s">
         <v>1246</v>
@@ -48627,7 +48626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -50352,115 +50351,115 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="19">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W4 W6:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>W5:X5 V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>X1:X4 X6:X1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H13 H16:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I13 I16:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J13 J16:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K13 K16:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$40</xm:f>
           </x14:formula1>
           <xm:sqref>H14:H15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>I14:I15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$3:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J14:J15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$11:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K14:K15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000010000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>L1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000011000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000012000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -50473,7 +50472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -51875,19 +51874,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H38 H41:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>H39:H40</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0200-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
@@ -51900,7 +51899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L107"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -53043,20 +53042,20 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F23" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J15 J18:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -53069,7 +53068,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -54157,13 +54156,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H2 H17:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -54176,7 +54175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -54835,7 +54834,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
@@ -54848,7 +54847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S381"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -57433,37 +57432,37 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0600-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$L$2:$L$3</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
@@ -57476,7 +57475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -59883,49 +59882,49 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -59938,7 +59937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -60704,19 +60703,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
added altimeter Valeport VA500 87405 to Instruments.xlsx and also changed previous altimeter 71991 to be a Valeport VA500
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3962" uniqueCount="1287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="1288">
   <si>
     <t>Model</t>
   </si>
@@ -4502,7 +4502,10 @@
     <t>Number of scans per bin</t>
   </si>
   <si>
-    <t>53447, 71991, 1251</t>
+    <t>87405, 71991</t>
+  </si>
+  <si>
+    <t>53447, 1251</t>
   </si>
 </sst>
 </file>
@@ -4988,7 +4991,7 @@
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="366">
+  <cellXfs count="364">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5917,10 +5920,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -47517,12 +47516,12 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H22:H23"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -47662,7 +47661,7 @@
       <c r="B3" s="89" t="s">
         <v>1256</v>
       </c>
-      <c r="F3" s="362"/>
+      <c r="F3" s="360"/>
       <c r="G3" s="183"/>
       <c r="H3" s="183"/>
       <c r="I3" s="349" t="s">
@@ -47709,7 +47708,7 @@
       <c r="E4" s="89" t="s">
         <v>1138</v>
       </c>
-      <c r="F4" s="362" t="s">
+      <c r="F4" s="360" t="s">
         <v>1139</v>
       </c>
       <c r="G4" s="183" t="s">
@@ -47762,13 +47761,13 @@
       <c r="E5" s="89" t="s">
         <v>1147</v>
       </c>
-      <c r="F5" s="362" t="s">
+      <c r="F5" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G5" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H5" s="363">
+      <c r="H5" s="361">
         <v>6164</v>
       </c>
       <c r="I5" s="349" t="s">
@@ -47806,7 +47805,7 @@
       <c r="B6" s="89" t="s">
         <v>1234</v>
       </c>
-      <c r="F6" s="362" t="s">
+      <c r="F6" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G6" s="349" t="s">
@@ -47852,13 +47851,13 @@
       <c r="B7" s="89" t="s">
         <v>1234</v>
       </c>
-      <c r="F7" s="362" t="s">
+      <c r="F7" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G7" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H7" s="363">
+      <c r="H7" s="361">
         <v>6164</v>
       </c>
       <c r="I7" s="349" t="s">
@@ -47897,7 +47896,7 @@
       <c r="B8" s="89" t="s">
         <v>1235</v>
       </c>
-      <c r="F8" s="362"/>
+      <c r="F8" s="360"/>
       <c r="G8" s="183"/>
       <c r="H8" s="359"/>
       <c r="I8" s="349" t="s">
@@ -47918,9 +47917,9 @@
       <c r="N8" s="359" t="s">
         <v>1161</v>
       </c>
-      <c r="O8" s="364"/>
-      <c r="P8" s="364"/>
-      <c r="Q8" s="364"/>
+      <c r="O8" s="362"/>
+      <c r="P8" s="362"/>
+      <c r="Q8" s="362"/>
       <c r="R8" s="183" t="s">
         <v>1162</v>
       </c>
@@ -47937,10 +47936,10 @@
       <c r="B9" s="89" t="s">
         <v>1231</v>
       </c>
-      <c r="F9" s="362" t="s">
+      <c r="F9" s="360" t="s">
         <v>1137</v>
       </c>
-      <c r="G9" s="362" t="s">
+      <c r="G9" s="360" t="s">
         <v>647</v>
       </c>
       <c r="H9" s="359" t="s">
@@ -47960,7 +47959,7 @@
       <c r="N9" s="359" t="s">
         <v>1164</v>
       </c>
-      <c r="O9" s="365" t="s">
+      <c r="O9" s="363" t="s">
         <v>1165</v>
       </c>
       <c r="P9" s="183" t="s">
@@ -47983,13 +47982,13 @@
       <c r="B10" s="89" t="s">
         <v>1231</v>
       </c>
-      <c r="F10" s="362" t="s">
+      <c r="F10" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G10" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H10" s="363">
+      <c r="H10" s="361">
         <v>6164</v>
       </c>
       <c r="I10" s="349" t="s">
@@ -48029,10 +48028,10 @@
       <c r="B11" s="89" t="s">
         <v>1232</v>
       </c>
-      <c r="F11" s="362" t="s">
+      <c r="F11" s="360" t="s">
         <v>1137</v>
       </c>
-      <c r="G11" s="362" t="s">
+      <c r="G11" s="360" t="s">
         <v>174</v>
       </c>
       <c r="H11" s="359" t="s">
@@ -48077,7 +48076,7 @@
       <c r="B12" s="183" t="s">
         <v>1266</v>
       </c>
-      <c r="F12" s="362"/>
+      <c r="F12" s="360"/>
       <c r="G12" s="183"/>
       <c r="H12" s="359"/>
       <c r="I12" s="349" t="s">
@@ -48110,10 +48109,10 @@
       <c r="B13" s="183" t="s">
         <v>1236</v>
       </c>
-      <c r="F13" s="362" t="s">
+      <c r="F13" s="360" t="s">
         <v>1177</v>
       </c>
-      <c r="G13" s="362" t="s">
+      <c r="G13" s="360" t="s">
         <v>1178</v>
       </c>
       <c r="H13" s="359" t="s">
@@ -48291,7 +48290,7 @@
         <v>571</v>
       </c>
       <c r="H17" s="359" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>574</v>
@@ -48319,38 +48318,42 @@
       <c r="V17" s="183"/>
       <c r="W17" s="183"/>
     </row>
-    <row r="18" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="183" t="s">
-        <v>1199</v>
+        <v>574</v>
       </c>
       <c r="B18" s="183" t="s">
-        <v>1259</v>
-      </c>
-      <c r="F18" s="362"/>
-      <c r="G18" s="183"/>
-      <c r="H18" s="183"/>
+        <v>1239</v>
+      </c>
+      <c r="F18" s="183" t="s">
+        <v>712</v>
+      </c>
+      <c r="G18" s="183" t="s">
+        <v>713</v>
+      </c>
+      <c r="H18" s="359" t="s">
+        <v>1286</v>
+      </c>
       <c r="I18" s="53" t="s">
-        <v>1200</v>
+        <v>574</v>
       </c>
       <c r="J18" s="354" t="s">
-        <v>1201</v>
+        <v>1195</v>
       </c>
       <c r="K18" s="354" t="s">
-        <v>1254</v>
-      </c>
-      <c r="L18" s="89" t="s">
-        <v>38</v>
-      </c>
-      <c r="M18" s="89" t="s">
-        <v>1202</v>
-      </c>
-      <c r="N18" s="359"/>
-      <c r="O18" s="183"/>
-      <c r="P18" s="183"/>
+        <v>1253</v>
+      </c>
+      <c r="N18" s="359" t="s">
+        <v>1196</v>
+      </c>
+      <c r="O18" s="183" t="s">
+        <v>1197</v>
+      </c>
+      <c r="P18" s="183" t="s">
+        <v>1198</v>
+      </c>
       <c r="Q18" s="183"/>
-      <c r="R18" s="183" t="s">
-        <v>1203</v>
-      </c>
+      <c r="R18" s="183"/>
       <c r="S18" s="183"/>
       <c r="T18" s="183"/>
       <c r="U18" s="183"/>
@@ -48359,26 +48362,36 @@
     </row>
     <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="183" t="s">
-        <v>1285</v>
+        <v>1199</v>
       </c>
       <c r="B19" s="183" t="s">
-        <v>1284</v>
-      </c>
-      <c r="F19" s="362"/>
+        <v>1259</v>
+      </c>
+      <c r="F19" s="360"/>
       <c r="G19" s="183"/>
       <c r="H19" s="183"/>
       <c r="I19" s="53" t="s">
-        <v>1283</v>
+        <v>1200</v>
       </c>
       <c r="J19" s="354" t="s">
-        <v>1282</v>
-      </c>
-      <c r="K19" s="354"/>
+        <v>1201</v>
+      </c>
+      <c r="K19" s="354" t="s">
+        <v>1254</v>
+      </c>
+      <c r="L19" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="M19" s="89" t="s">
+        <v>1202</v>
+      </c>
       <c r="N19" s="359"/>
       <c r="O19" s="183"/>
       <c r="P19" s="183"/>
       <c r="Q19" s="183"/>
-      <c r="R19" s="183"/>
+      <c r="R19" s="183" t="s">
+        <v>1203</v>
+      </c>
       <c r="S19" s="183"/>
       <c r="T19" s="183"/>
       <c r="U19" s="183"/>
@@ -48387,21 +48400,21 @@
     </row>
     <row r="20" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="183" t="s">
-        <v>1204</v>
+        <v>1285</v>
       </c>
       <c r="B20" s="183" t="s">
-        <v>1258</v>
-      </c>
-      <c r="F20" s="362"/>
+        <v>1284</v>
+      </c>
+      <c r="F20" s="360"/>
       <c r="G20" s="183"/>
       <c r="H20" s="183"/>
-      <c r="I20" s="89" t="s">
-        <v>1205</v>
-      </c>
-      <c r="J20" s="348" t="s">
-        <v>1206</v>
-      </c>
-      <c r="K20" s="348"/>
+      <c r="I20" s="53" t="s">
+        <v>1283</v>
+      </c>
+      <c r="J20" s="354" t="s">
+        <v>1282</v>
+      </c>
+      <c r="K20" s="354"/>
       <c r="N20" s="359"/>
       <c r="O20" s="183"/>
       <c r="P20" s="183"/>
@@ -48415,29 +48428,25 @@
     </row>
     <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="183" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B21" s="183" t="s">
-        <v>1260</v>
-      </c>
-      <c r="F21" s="362" t="s">
-        <v>1137</v>
-      </c>
-      <c r="G21" s="183" t="s">
-        <v>1208</v>
-      </c>
+        <v>1258</v>
+      </c>
+      <c r="F21" s="360"/>
+      <c r="G21" s="183"/>
       <c r="H21" s="183"/>
       <c r="I21" s="89" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="J21" s="348" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="K21" s="348"/>
       <c r="N21" s="359"/>
-      <c r="O21" s="359"/>
-      <c r="P21" s="359"/>
-      <c r="Q21" s="359"/>
+      <c r="O21" s="183"/>
+      <c r="P21" s="183"/>
+      <c r="Q21" s="183"/>
       <c r="R21" s="183"/>
       <c r="S21" s="183"/>
       <c r="T21" s="183"/>
@@ -48445,38 +48454,32 @@
       <c r="V21" s="183"/>
       <c r="W21" s="183"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="183" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="B22" s="183" t="s">
-        <v>1279</v>
-      </c>
-      <c r="F22" s="183"/>
-      <c r="G22" s="183"/>
+        <v>1260</v>
+      </c>
+      <c r="F22" s="360" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G22" s="183" t="s">
+        <v>1208</v>
+      </c>
       <c r="H22" s="183"/>
       <c r="I22" s="89" t="s">
-        <v>1225</v>
-      </c>
-      <c r="J22" s="354" t="s">
-        <v>1280</v>
-      </c>
-      <c r="K22" s="354" t="s">
-        <v>1255</v>
-      </c>
-      <c r="L22" s="89" t="s">
-        <v>38</v>
-      </c>
-      <c r="M22" s="89" t="s">
-        <v>1160</v>
-      </c>
+        <v>1209</v>
+      </c>
+      <c r="J22" s="348" t="s">
+        <v>1210</v>
+      </c>
+      <c r="K22" s="348"/>
       <c r="N22" s="359"/>
-      <c r="O22" s="183"/>
-      <c r="P22" s="183"/>
-      <c r="Q22" s="183"/>
-      <c r="R22" s="183" t="s">
-        <v>1212</v>
-      </c>
+      <c r="O22" s="359"/>
+      <c r="P22" s="359"/>
+      <c r="Q22" s="359"/>
+      <c r="R22" s="183"/>
       <c r="S22" s="183"/>
       <c r="T22" s="183"/>
       <c r="U22" s="183"/>
@@ -48488,7 +48491,7 @@
         <v>1211</v>
       </c>
       <c r="B23" s="183" t="s">
-        <v>1274</v>
+        <v>1279</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
@@ -48497,7 +48500,7 @@
         <v>1225</v>
       </c>
       <c r="J23" s="354" t="s">
-        <v>1275</v>
+        <v>1280</v>
       </c>
       <c r="K23" s="354" t="s">
         <v>1255</v>
@@ -48523,28 +48526,28 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="183" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="B24" s="183" t="s">
-        <v>1257</v>
+        <v>1274</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
       <c r="H24" s="183"/>
       <c r="I24" s="89" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="J24" s="354" t="s">
-        <v>1219</v>
+        <v>1275</v>
       </c>
       <c r="K24" s="354" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="L24" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M24" s="89" t="s">
-        <v>1214</v>
+        <v>1160</v>
       </c>
       <c r="N24" s="359"/>
       <c r="O24" s="183"/>
@@ -48561,31 +48564,36 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="183" t="s">
-        <v>1267</v>
+        <v>1213</v>
       </c>
       <c r="B25" s="183" t="s">
-        <v>1268</v>
+        <v>1257</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
       <c r="H25" s="183"/>
-      <c r="I25" s="360" t="s">
-        <v>1269</v>
+      <c r="I25" s="89" t="s">
+        <v>1226</v>
       </c>
       <c r="J25" s="354" t="s">
-        <v>1277</v>
+        <v>1219</v>
       </c>
       <c r="K25" s="354" t="s">
-        <v>1245</v>
-      </c>
-      <c r="L25" s="360" t="s">
+        <v>1254</v>
+      </c>
+      <c r="L25" s="183" t="s">
         <v>38</v>
       </c>
-      <c r="N25" s="183"/>
+      <c r="M25" s="89" t="s">
+        <v>1214</v>
+      </c>
+      <c r="N25" s="359"/>
       <c r="O25" s="183"/>
       <c r="P25" s="183"/>
       <c r="Q25" s="183"/>
-      <c r="R25" s="183"/>
+      <c r="R25" s="183" t="s">
+        <v>1212</v>
+      </c>
       <c r="S25" s="183"/>
       <c r="T25" s="183"/>
       <c r="U25" s="183"/>
@@ -48594,30 +48602,63 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="183" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="B26" s="183" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="F26" s="183"/>
       <c r="G26" s="183"/>
       <c r="H26" s="183"/>
-      <c r="I26" s="361" t="s">
-        <v>1272</v>
-      </c>
-      <c r="J26" s="348" t="s">
-        <v>1278</v>
-      </c>
-      <c r="K26" s="348" t="s">
-        <v>1246</v>
-      </c>
-      <c r="L26" s="361" t="s">
+      <c r="I26" s="349" t="s">
+        <v>1269</v>
+      </c>
+      <c r="J26" s="354" t="s">
+        <v>1277</v>
+      </c>
+      <c r="K26" s="354" t="s">
+        <v>1245</v>
+      </c>
+      <c r="L26" s="349" t="s">
         <v>38</v>
       </c>
       <c r="N26" s="183"/>
       <c r="O26" s="183"/>
       <c r="P26" s="183"/>
       <c r="Q26" s="183"/>
+      <c r="R26" s="183"/>
+      <c r="S26" s="183"/>
+      <c r="T26" s="183"/>
+      <c r="U26" s="183"/>
+      <c r="V26" s="183"/>
+      <c r="W26" s="183"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A27" s="183" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B27" s="183" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F27" s="183"/>
+      <c r="G27" s="183"/>
+      <c r="H27" s="183"/>
+      <c r="I27" s="183" t="s">
+        <v>1272</v>
+      </c>
+      <c r="J27" s="348" t="s">
+        <v>1278</v>
+      </c>
+      <c r="K27" s="348" t="s">
+        <v>1246</v>
+      </c>
+      <c r="L27" s="183" t="s">
+        <v>38</v>
+      </c>
+      <c r="N27" s="183"/>
+      <c r="O27" s="183"/>
+      <c r="P27" s="183"/>
+      <c r="Q27" s="183"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added all sensors on UMF 6929 SBE19 /MHAN
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20402"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F378A945-A0D8-4B2E-A7A2-F950D9086C5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18"/>
+    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SBE MicroCATs" sheetId="1" r:id="rId1"/>
@@ -57,12 +58,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -91,12 +92,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ocean.gbg11</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -147,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000003000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000004000000}">
       <text>
         <r>
           <rPr>
@@ -203,12 +204,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -237,12 +238,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -271,12 +272,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -305,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="1289">
   <si>
     <t>Model</t>
   </si>
@@ -4178,9 +4179,6 @@
     <t>Biospherical</t>
   </si>
   <si>
-    <t>QSP-2000</t>
-  </si>
-  <si>
     <t>PAR</t>
   </si>
   <si>
@@ -4439,9 +4437,6 @@
     <t>Klorofyllfluorescens*</t>
   </si>
   <si>
-    <t>70374, 70711</t>
-  </si>
-  <si>
     <t>sbeox0PS, sbeox1PS</t>
   </si>
   <si>
@@ -4463,9 +4458,6 @@
     <t>Temperatur diff</t>
   </si>
   <si>
-    <t>FLNTURTD-2288, FLNTURT-115, FLNTURT-1899</t>
-  </si>
-  <si>
     <t>density00, density11</t>
   </si>
   <si>
@@ -4506,12 +4498,24 @@
   </si>
   <si>
     <t>53447, 1251</t>
+  </si>
+  <si>
+    <t>6164, 6929</t>
+  </si>
+  <si>
+    <t>70374, 70711, 70397</t>
+  </si>
+  <si>
+    <t>FLNTURTD-2288, FLNTURT-115, FLNTURT-1899, FLNTURT-2470</t>
+  </si>
+  <si>
+    <t>QSP-2000, QSP-2350</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
@@ -5928,12 +5932,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Förklarande text 2" xfId="4"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlänk 2" xfId="3"/>
+    <cellStyle name="Förklarande text 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlänk 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="1602">
     <dxf>
@@ -17642,7 +17646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -23664,79 +23668,79 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>W26:W1048576 W1:W17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576 W18:W25</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$23</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000B000000}">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>Listor!$M:$M</xm:f>
           </x14:formula1>
@@ -23749,7 +23753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -24703,25 +24707,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -24734,7 +24738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -25584,25 +25588,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -25615,7 +25619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -27210,19 +27214,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$45</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -27235,7 +27239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -29110,31 +29114,31 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$3:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$N$2:$N$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
@@ -29147,7 +29151,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -29159,7 +29163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AD100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -33173,73 +33177,73 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0E00-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>AA1:AA1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000002000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000003000000}">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000004000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000005000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000006000000}">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000007000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0E00-000008000000}">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
           <xm:sqref>Z1:Z1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej" xr:uid="{00000000-0002-0000-0E00-000009000000}">
           <x14:formula1>
             <xm:f>Listor!$M$3:$M$7</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000A000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000B000000}">
           <x14:formula1>
             <xm:f>Listor!$A:$A</xm:f>
           </x14:formula1>
@@ -33252,7 +33256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -45066,19 +45070,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -45091,7 +45095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -46919,19 +46923,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -46944,7 +46948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -47515,13 +47519,13 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -47547,7 +47551,7 @@
         <v>1099</v>
       </c>
       <c r="B1" s="345" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="C1" s="345" t="s">
         <v>390</v>
@@ -47574,7 +47578,7 @@
         <v>1106</v>
       </c>
       <c r="K1" s="345" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="L1" s="345" t="s">
         <v>1107</v>
@@ -47603,7 +47607,7 @@
         <v>1114</v>
       </c>
       <c r="B2" s="346" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C2" s="346" t="s">
         <v>1115</v>
@@ -47630,7 +47634,7 @@
         <v>1122</v>
       </c>
       <c r="K2" s="346" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="L2" s="346" t="s">
         <v>1123</v>
@@ -47659,7 +47663,7 @@
         <v>1130</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="F3" s="360"/>
       <c r="G3" s="183"/>
@@ -47671,7 +47675,7 @@
         <v>1132</v>
       </c>
       <c r="K3" s="348" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="L3" s="89" t="s">
         <v>38</v>
@@ -47697,7 +47701,7 @@
         <v>1135</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>1136</v>
@@ -47724,7 +47728,7 @@
         <v>1143</v>
       </c>
       <c r="K4" s="348" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="N4" s="359" t="s">
         <v>1144</v>
@@ -47750,7 +47754,7 @@
         <v>1135</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>1136</v>
@@ -47767,8 +47771,8 @@
       <c r="G5" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H5" s="361">
-        <v>6164</v>
+      <c r="H5" s="361" t="s">
+        <v>1285</v>
       </c>
       <c r="I5" s="349" t="s">
         <v>1142</v>
@@ -47777,7 +47781,7 @@
         <v>1143</v>
       </c>
       <c r="K5" s="348" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="N5" s="351"/>
       <c r="O5" s="352" t="s">
@@ -47803,7 +47807,7 @@
         <v>1152</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="F6" s="360" t="s">
         <v>1137</v>
@@ -47815,13 +47819,13 @@
         <v>1153</v>
       </c>
       <c r="I6" s="349" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="J6" s="354" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="K6" s="354" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="L6" s="355"/>
       <c r="M6" s="355"/>
@@ -47849,7 +47853,7 @@
         <v>1152</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="F7" s="360" t="s">
         <v>1137</v>
@@ -47857,17 +47861,17 @@
       <c r="G7" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H7" s="361">
-        <v>6164</v>
+      <c r="H7" s="361" t="s">
+        <v>1285</v>
       </c>
       <c r="I7" s="349" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="J7" s="354" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="K7" s="354" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="L7" s="356"/>
       <c r="N7" s="183"/>
@@ -47894,19 +47898,19 @@
         <v>1159</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="F8" s="360"/>
       <c r="G8" s="183"/>
       <c r="H8" s="359"/>
       <c r="I8" s="349" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="J8" s="348" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="K8" s="348" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="L8" s="89" t="s">
         <v>38</v>
@@ -47934,7 +47938,7 @@
         <v>1163</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F9" s="360" t="s">
         <v>1137</v>
@@ -47943,16 +47947,16 @@
         <v>647</v>
       </c>
       <c r="H9" s="359" t="s">
-        <v>1281</v>
+        <v>1278</v>
       </c>
       <c r="I9" s="349" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J9" s="348" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K9" s="348" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="L9" s="350"/>
       <c r="M9" s="350"/>
@@ -47980,7 +47984,7 @@
         <v>1163</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F10" s="360" t="s">
         <v>1137</v>
@@ -47988,17 +47992,17 @@
       <c r="G10" s="183" t="s">
         <v>1148</v>
       </c>
-      <c r="H10" s="361">
-        <v>6164</v>
+      <c r="H10" s="361" t="s">
+        <v>1285</v>
       </c>
       <c r="I10" s="349" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J10" s="348" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K10" s="348" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="L10" s="350"/>
       <c r="M10" s="356"/>
@@ -48023,10 +48027,10 @@
     </row>
     <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F11" s="360" t="s">
         <v>1137</v>
@@ -48038,13 +48042,13 @@
         <v>1170</v>
       </c>
       <c r="I11" s="349" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="J11" s="348" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="K11" s="348" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="L11" s="350"/>
       <c r="M11" s="350"/>
@@ -48074,19 +48078,19 @@
         <v>1175</v>
       </c>
       <c r="B12" s="183" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="F12" s="360"/>
       <c r="G12" s="183"/>
       <c r="H12" s="359"/>
       <c r="I12" s="349" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J12" s="348" t="s">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="K12" s="348" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="L12" s="89" t="s">
         <v>38</v>
@@ -48107,33 +48111,33 @@
         <v>1176</v>
       </c>
       <c r="B13" s="183" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F13" s="360" t="s">
         <v>1177</v>
       </c>
       <c r="G13" s="360" t="s">
+        <v>1288</v>
+      </c>
+      <c r="H13" s="359" t="s">
+        <v>1286</v>
+      </c>
+      <c r="I13" s="89" t="s">
         <v>1178</v>
       </c>
-      <c r="H13" s="359" t="s">
-        <v>1265</v>
-      </c>
-      <c r="I13" s="89" t="s">
+      <c r="J13" s="348" t="s">
         <v>1179</v>
       </c>
-      <c r="J13" s="348" t="s">
-        <v>1180</v>
-      </c>
       <c r="K13" s="348" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="L13" s="350"/>
       <c r="M13" s="350"/>
       <c r="N13" s="359" t="s">
+        <v>1180</v>
+      </c>
+      <c r="O13" s="183" t="s">
         <v>1181</v>
-      </c>
-      <c r="O13" s="183" t="s">
-        <v>1182</v>
       </c>
       <c r="P13" s="183"/>
       <c r="Q13" s="183"/>
@@ -48146,37 +48150,37 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="183" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B14" s="183" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="F14" s="183" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G14" s="183" t="s">
         <v>1183</v>
       </c>
-      <c r="G14" s="183" t="s">
-        <v>1184</v>
-      </c>
       <c r="H14" s="359" t="s">
-        <v>1273</v>
+        <v>1287</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="J14" s="354" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="K14" s="354" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="N14" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O14" s="183" t="s">
+        <v>1184</v>
+      </c>
+      <c r="P14" s="183" t="s">
         <v>1185</v>
-      </c>
-      <c r="P14" s="183" t="s">
-        <v>1186</v>
       </c>
       <c r="Q14" s="183">
         <v>8</v>
@@ -48190,37 +48194,37 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="183" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B15" s="183" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="F15" s="183" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G15" s="183" t="s">
         <v>1183</v>
       </c>
-      <c r="G15" s="183" t="s">
-        <v>1184</v>
-      </c>
       <c r="H15" s="359" t="s">
-        <v>1273</v>
+        <v>1287</v>
       </c>
       <c r="I15" s="53" t="s">
+        <v>1186</v>
+      </c>
+      <c r="J15" s="354" t="s">
         <v>1187</v>
       </c>
-      <c r="J15" s="354" t="s">
-        <v>1188</v>
-      </c>
       <c r="K15" s="354" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="N15" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O15" s="183" t="s">
+        <v>1188</v>
+      </c>
+      <c r="P15" s="183" t="s">
         <v>1189</v>
-      </c>
-      <c r="P15" s="183" t="s">
-        <v>1190</v>
       </c>
       <c r="Q15" s="183">
         <v>8</v>
@@ -48234,37 +48238,37 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="183" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B16" s="183" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="F16" s="183" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="G16" s="183" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="H16" s="359" t="s">
         <v>235</v>
       </c>
       <c r="I16" s="53" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="J16" s="354" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="K16" s="354" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="N16" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O16" s="183" t="s">
+        <v>1191</v>
+      </c>
+      <c r="P16" s="183" t="s">
         <v>1192</v>
-      </c>
-      <c r="P16" s="183" t="s">
-        <v>1193</v>
       </c>
       <c r="Q16" s="183">
         <v>8</v>
@@ -48281,34 +48285,34 @@
         <v>574</v>
       </c>
       <c r="B17" s="183" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="F17" s="183" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="G17" s="183" t="s">
         <v>571</v>
       </c>
       <c r="H17" s="359" t="s">
-        <v>1287</v>
+        <v>1284</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J17" s="354" t="s">
+        <v>1194</v>
+      </c>
+      <c r="K17" s="354" t="s">
+        <v>1252</v>
+      </c>
+      <c r="N17" s="359" t="s">
         <v>1195</v>
       </c>
-      <c r="K17" s="354" t="s">
-        <v>1253</v>
-      </c>
-      <c r="N17" s="359" t="s">
+      <c r="O17" s="183" t="s">
         <v>1196</v>
       </c>
-      <c r="O17" s="183" t="s">
+      <c r="P17" s="183" t="s">
         <v>1197</v>
-      </c>
-      <c r="P17" s="183" t="s">
-        <v>1198</v>
       </c>
       <c r="Q17" s="183"/>
       <c r="R17" s="183"/>
@@ -48323,7 +48327,7 @@
         <v>574</v>
       </c>
       <c r="B18" s="183" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="F18" s="183" t="s">
         <v>712</v>
@@ -48332,25 +48336,25 @@
         <v>713</v>
       </c>
       <c r="H18" s="359" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J18" s="354" t="s">
+        <v>1194</v>
+      </c>
+      <c r="K18" s="354" t="s">
+        <v>1252</v>
+      </c>
+      <c r="N18" s="359" t="s">
         <v>1195</v>
       </c>
-      <c r="K18" s="354" t="s">
-        <v>1253</v>
-      </c>
-      <c r="N18" s="359" t="s">
+      <c r="O18" s="183" t="s">
         <v>1196</v>
       </c>
-      <c r="O18" s="183" t="s">
+      <c r="P18" s="183" t="s">
         <v>1197</v>
-      </c>
-      <c r="P18" s="183" t="s">
-        <v>1198</v>
       </c>
       <c r="Q18" s="183"/>
       <c r="R18" s="183"/>
@@ -48362,35 +48366,35 @@
     </row>
     <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="183" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B19" s="183" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="F19" s="360"/>
       <c r="G19" s="183"/>
       <c r="H19" s="183"/>
       <c r="I19" s="53" t="s">
+        <v>1199</v>
+      </c>
+      <c r="J19" s="354" t="s">
         <v>1200</v>
       </c>
-      <c r="J19" s="354" t="s">
-        <v>1201</v>
-      </c>
       <c r="K19" s="354" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="L19" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M19" s="89" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="N19" s="359"/>
       <c r="O19" s="183"/>
       <c r="P19" s="183"/>
       <c r="Q19" s="183"/>
       <c r="R19" s="183" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="S19" s="183"/>
       <c r="T19" s="183"/>
@@ -48400,19 +48404,19 @@
     </row>
     <row r="20" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="183" t="s">
-        <v>1285</v>
+        <v>1282</v>
       </c>
       <c r="B20" s="183" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="F20" s="360"/>
       <c r="G20" s="183"/>
       <c r="H20" s="183"/>
       <c r="I20" s="53" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="J20" s="354" t="s">
-        <v>1282</v>
+        <v>1279</v>
       </c>
       <c r="K20" s="354"/>
       <c r="N20" s="359"/>
@@ -48428,19 +48432,19 @@
     </row>
     <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="183" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B21" s="183" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F21" s="360"/>
       <c r="G21" s="183"/>
       <c r="H21" s="183"/>
       <c r="I21" s="89" t="s">
+        <v>1204</v>
+      </c>
+      <c r="J21" s="348" t="s">
         <v>1205</v>
-      </c>
-      <c r="J21" s="348" t="s">
-        <v>1206</v>
       </c>
       <c r="K21" s="348"/>
       <c r="N21" s="359"/>
@@ -48456,23 +48460,23 @@
     </row>
     <row r="22" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="183" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B22" s="183" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="F22" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G22" s="183" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="H22" s="183"/>
       <c r="I22" s="89" t="s">
+        <v>1208</v>
+      </c>
+      <c r="J22" s="348" t="s">
         <v>1209</v>
-      </c>
-      <c r="J22" s="348" t="s">
-        <v>1210</v>
       </c>
       <c r="K22" s="348"/>
       <c r="N22" s="359"/>
@@ -48488,22 +48492,22 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="183" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B23" s="183" t="s">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
       <c r="H23" s="183"/>
       <c r="I23" s="89" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="J23" s="354" t="s">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="K23" s="354" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="L23" s="89" t="s">
         <v>38</v>
@@ -48516,7 +48520,7 @@
       <c r="P23" s="183"/>
       <c r="Q23" s="183"/>
       <c r="R23" s="183" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="S23" s="183"/>
       <c r="T23" s="183"/>
@@ -48526,22 +48530,22 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="183" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B24" s="183" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
       <c r="H24" s="183"/>
       <c r="I24" s="89" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="J24" s="354" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="K24" s="354" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="L24" s="89" t="s">
         <v>38</v>
@@ -48554,7 +48558,7 @@
       <c r="P24" s="183"/>
       <c r="Q24" s="183"/>
       <c r="R24" s="183" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="S24" s="183"/>
       <c r="T24" s="183"/>
@@ -48564,35 +48568,35 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="183" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B25" s="183" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
       <c r="H25" s="183"/>
       <c r="I25" s="89" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="J25" s="354" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K25" s="354" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="L25" s="183" t="s">
         <v>38</v>
       </c>
       <c r="M25" s="89" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="N25" s="359"/>
       <c r="O25" s="183"/>
       <c r="P25" s="183"/>
       <c r="Q25" s="183"/>
       <c r="R25" s="183" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="S25" s="183"/>
       <c r="T25" s="183"/>
@@ -48602,22 +48606,22 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="183" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="B26" s="183" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="F26" s="183"/>
       <c r="G26" s="183"/>
       <c r="H26" s="183"/>
       <c r="I26" s="349" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="J26" s="354" t="s">
-        <v>1277</v>
+        <v>1274</v>
       </c>
       <c r="K26" s="354" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="L26" s="349" t="s">
         <v>38</v>
@@ -48635,22 +48639,22 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="183" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B27" s="183" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="F27" s="183"/>
       <c r="G27" s="183"/>
       <c r="H27" s="183"/>
       <c r="I27" s="183" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="J27" s="348" t="s">
-        <v>1278</v>
+        <v>1275</v>
       </c>
       <c r="K27" s="348" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="L27" s="183" t="s">
         <v>38</v>
@@ -48667,7 +48671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -50392,115 +50396,115 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="19">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W4 W6:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>W5:X5 V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>X1:X4 X6:X1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H13 H16:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I13 I16:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J13 J16:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K13 K16:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$40</xm:f>
           </x14:formula1>
           <xm:sqref>H14:H15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>I14:I15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$3:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J14:J15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$11:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K14:K15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000010000000}">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>L1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000011000000}">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000012000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -50513,7 +50517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -51915,19 +51919,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H38 H41:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>H39:H40</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
@@ -51940,7 +51944,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -53083,20 +53087,20 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1"/>
+    <hyperlink ref="F23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J15 J18:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -53109,7 +53113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -54197,13 +54201,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H2 H17:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -54216,7 +54220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -54875,7 +54879,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
@@ -54888,7 +54892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S381"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -57473,37 +57477,37 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$L$2:$L$3</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000005000000}">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
@@ -57516,7 +57520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -59923,49 +59927,49 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000005000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000006000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000007000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -59978,7 +59982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -60744,19 +60748,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Added more SBE19 specific param names to be able to create std-format files /Mhan
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F378A945-A0D8-4B2E-A7A2-F950D9086C5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEE97D6-D240-4F30-A99F-076C7EA16A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="1291">
   <si>
     <t>Model</t>
   </si>
@@ -4173,9 +4173,6 @@
     <t>Oxygen, SBE 43 [% saturation]</t>
   </si>
   <si>
-    <t>PAR/Irradiance, Biospherical/Licor</t>
-  </si>
-  <si>
     <t>Biospherical</t>
   </si>
   <si>
@@ -4510,6 +4507,15 @@
   </si>
   <si>
     <t>QSP-2000, QSP-2350</t>
+  </si>
+  <si>
+    <t>tv290C</t>
+  </si>
+  <si>
+    <t>prdM</t>
+  </si>
+  <si>
+    <t>PAR/Irradiance, PAR/Irradiance, Biospherical/Lico, Biospherical/Licor</t>
   </si>
 </sst>
 </file>
@@ -47525,7 +47531,7 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -47551,7 +47557,7 @@
         <v>1099</v>
       </c>
       <c r="B1" s="345" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C1" s="345" t="s">
         <v>390</v>
@@ -47578,7 +47584,7 @@
         <v>1106</v>
       </c>
       <c r="K1" s="345" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="L1" s="345" t="s">
         <v>1107</v>
@@ -47607,7 +47613,7 @@
         <v>1114</v>
       </c>
       <c r="B2" s="346" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C2" s="346" t="s">
         <v>1115</v>
@@ -47634,7 +47640,7 @@
         <v>1122</v>
       </c>
       <c r="K2" s="346" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="L2" s="346" t="s">
         <v>1123</v>
@@ -47663,7 +47669,7 @@
         <v>1130</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="F3" s="360"/>
       <c r="G3" s="183"/>
@@ -47675,7 +47681,7 @@
         <v>1132</v>
       </c>
       <c r="K3" s="348" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="L3" s="89" t="s">
         <v>38</v>
@@ -47701,7 +47707,7 @@
         <v>1135</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>1136</v>
@@ -47728,7 +47734,7 @@
         <v>1143</v>
       </c>
       <c r="K4" s="348" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="N4" s="359" t="s">
         <v>1144</v>
@@ -47754,7 +47760,7 @@
         <v>1135</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>1232</v>
+        <v>1289</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>1136</v>
@@ -47772,7 +47778,7 @@
         <v>1148</v>
       </c>
       <c r="H5" s="361" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="I5" s="349" t="s">
         <v>1142</v>
@@ -47781,7 +47787,7 @@
         <v>1143</v>
       </c>
       <c r="K5" s="348" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="N5" s="351"/>
       <c r="O5" s="352" t="s">
@@ -47807,7 +47813,7 @@
         <v>1152</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="F6" s="360" t="s">
         <v>1137</v>
@@ -47819,13 +47825,13 @@
         <v>1153</v>
       </c>
       <c r="I6" s="349" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="J6" s="354" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="K6" s="354" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="L6" s="355"/>
       <c r="M6" s="355"/>
@@ -47853,7 +47859,7 @@
         <v>1152</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="F7" s="360" t="s">
         <v>1137</v>
@@ -47862,16 +47868,16 @@
         <v>1148</v>
       </c>
       <c r="H7" s="361" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="I7" s="349" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="J7" s="354" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="K7" s="354" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="L7" s="356"/>
       <c r="N7" s="183"/>
@@ -47898,19 +47904,19 @@
         <v>1159</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="F8" s="360"/>
       <c r="G8" s="183"/>
       <c r="H8" s="359"/>
       <c r="I8" s="349" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="J8" s="348" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="K8" s="348" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="L8" s="89" t="s">
         <v>38</v>
@@ -47938,7 +47944,7 @@
         <v>1163</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="F9" s="360" t="s">
         <v>1137</v>
@@ -47947,16 +47953,16 @@
         <v>647</v>
       </c>
       <c r="H9" s="359" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="I9" s="349" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="J9" s="348" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="K9" s="348" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="L9" s="350"/>
       <c r="M9" s="350"/>
@@ -47984,7 +47990,7 @@
         <v>1163</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>1230</v>
+        <v>1288</v>
       </c>
       <c r="F10" s="360" t="s">
         <v>1137</v>
@@ -47993,16 +47999,16 @@
         <v>1148</v>
       </c>
       <c r="H10" s="361" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="I10" s="349" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="J10" s="348" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="K10" s="348" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="L10" s="350"/>
       <c r="M10" s="356"/>
@@ -48027,10 +48033,10 @@
     </row>
     <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F11" s="360" t="s">
         <v>1137</v>
@@ -48042,13 +48048,13 @@
         <v>1170</v>
       </c>
       <c r="I11" s="349" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J11" s="348" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K11" s="348" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="L11" s="350"/>
       <c r="M11" s="350"/>
@@ -48078,19 +48084,19 @@
         <v>1175</v>
       </c>
       <c r="B12" s="183" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="F12" s="360"/>
       <c r="G12" s="183"/>
       <c r="H12" s="359"/>
       <c r="I12" s="349" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="J12" s="348" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="K12" s="348" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="L12" s="89" t="s">
         <v>38</v>
@@ -48108,36 +48114,36 @@
     </row>
     <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="183" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B13" s="183" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F13" s="360" t="s">
         <v>1176</v>
       </c>
-      <c r="B13" s="183" t="s">
-        <v>1235</v>
-      </c>
-      <c r="F13" s="360" t="s">
+      <c r="G13" s="360" t="s">
+        <v>1287</v>
+      </c>
+      <c r="H13" s="359" t="s">
+        <v>1285</v>
+      </c>
+      <c r="I13" s="89" t="s">
         <v>1177</v>
       </c>
-      <c r="G13" s="360" t="s">
-        <v>1288</v>
-      </c>
-      <c r="H13" s="359" t="s">
-        <v>1286</v>
-      </c>
-      <c r="I13" s="89" t="s">
+      <c r="J13" s="348" t="s">
         <v>1178</v>
       </c>
-      <c r="J13" s="348" t="s">
-        <v>1179</v>
-      </c>
       <c r="K13" s="348" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="L13" s="350"/>
       <c r="M13" s="350"/>
       <c r="N13" s="359" t="s">
+        <v>1179</v>
+      </c>
+      <c r="O13" s="183" t="s">
         <v>1180</v>
-      </c>
-      <c r="O13" s="183" t="s">
-        <v>1181</v>
       </c>
       <c r="P13" s="183"/>
       <c r="Q13" s="183"/>
@@ -48150,37 +48156,37 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="183" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B14" s="183" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F14" s="183" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G14" s="183" t="s">
         <v>1182</v>
       </c>
-      <c r="G14" s="183" t="s">
-        <v>1183</v>
-      </c>
       <c r="H14" s="359" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J14" s="354" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="K14" s="354" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="N14" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O14" s="183" t="s">
+        <v>1183</v>
+      </c>
+      <c r="P14" s="183" t="s">
         <v>1184</v>
-      </c>
-      <c r="P14" s="183" t="s">
-        <v>1185</v>
       </c>
       <c r="Q14" s="183">
         <v>8</v>
@@ -48194,37 +48200,37 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="183" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B15" s="183" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="F15" s="183" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G15" s="183" t="s">
         <v>1182</v>
       </c>
-      <c r="G15" s="183" t="s">
-        <v>1183</v>
-      </c>
       <c r="H15" s="359" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="I15" s="53" t="s">
+        <v>1185</v>
+      </c>
+      <c r="J15" s="354" t="s">
         <v>1186</v>
       </c>
-      <c r="J15" s="354" t="s">
-        <v>1187</v>
-      </c>
       <c r="K15" s="354" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="N15" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O15" s="183" t="s">
+        <v>1187</v>
+      </c>
+      <c r="P15" s="183" t="s">
         <v>1188</v>
-      </c>
-      <c r="P15" s="183" t="s">
-        <v>1189</v>
       </c>
       <c r="Q15" s="183">
         <v>8</v>
@@ -48238,37 +48244,37 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="183" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B16" s="183" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F16" s="183" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="G16" s="183" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="H16" s="359" t="s">
         <v>235</v>
       </c>
       <c r="I16" s="53" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="J16" s="354" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="K16" s="354" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="N16" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O16" s="183" t="s">
+        <v>1190</v>
+      </c>
+      <c r="P16" s="183" t="s">
         <v>1191</v>
-      </c>
-      <c r="P16" s="183" t="s">
-        <v>1192</v>
       </c>
       <c r="Q16" s="183">
         <v>8</v>
@@ -48285,34 +48291,34 @@
         <v>574</v>
       </c>
       <c r="B17" s="183" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="F17" s="183" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="G17" s="183" t="s">
         <v>571</v>
       </c>
       <c r="H17" s="359" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J17" s="354" t="s">
+        <v>1193</v>
+      </c>
+      <c r="K17" s="354" t="s">
+        <v>1251</v>
+      </c>
+      <c r="N17" s="359" t="s">
         <v>1194</v>
       </c>
-      <c r="K17" s="354" t="s">
-        <v>1252</v>
-      </c>
-      <c r="N17" s="359" t="s">
+      <c r="O17" s="183" t="s">
         <v>1195</v>
       </c>
-      <c r="O17" s="183" t="s">
+      <c r="P17" s="183" t="s">
         <v>1196</v>
-      </c>
-      <c r="P17" s="183" t="s">
-        <v>1197</v>
       </c>
       <c r="Q17" s="183"/>
       <c r="R17" s="183"/>
@@ -48327,7 +48333,7 @@
         <v>574</v>
       </c>
       <c r="B18" s="183" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="F18" s="183" t="s">
         <v>712</v>
@@ -48336,25 +48342,25 @@
         <v>713</v>
       </c>
       <c r="H18" s="359" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J18" s="354" t="s">
+        <v>1193</v>
+      </c>
+      <c r="K18" s="354" t="s">
+        <v>1251</v>
+      </c>
+      <c r="N18" s="359" t="s">
         <v>1194</v>
       </c>
-      <c r="K18" s="354" t="s">
-        <v>1252</v>
-      </c>
-      <c r="N18" s="359" t="s">
+      <c r="O18" s="183" t="s">
         <v>1195</v>
       </c>
-      <c r="O18" s="183" t="s">
+      <c r="P18" s="183" t="s">
         <v>1196</v>
-      </c>
-      <c r="P18" s="183" t="s">
-        <v>1197</v>
       </c>
       <c r="Q18" s="183"/>
       <c r="R18" s="183"/>
@@ -48366,35 +48372,35 @@
     </row>
     <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="183" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B19" s="183" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F19" s="360"/>
       <c r="G19" s="183"/>
       <c r="H19" s="183"/>
       <c r="I19" s="53" t="s">
+        <v>1198</v>
+      </c>
+      <c r="J19" s="354" t="s">
         <v>1199</v>
       </c>
-      <c r="J19" s="354" t="s">
-        <v>1200</v>
-      </c>
       <c r="K19" s="354" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="L19" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M19" s="89" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="N19" s="359"/>
       <c r="O19" s="183"/>
       <c r="P19" s="183"/>
       <c r="Q19" s="183"/>
       <c r="R19" s="183" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="S19" s="183"/>
       <c r="T19" s="183"/>
@@ -48404,19 +48410,19 @@
     </row>
     <row r="20" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="183" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B20" s="183" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F20" s="360"/>
       <c r="G20" s="183"/>
       <c r="H20" s="183"/>
       <c r="I20" s="53" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="J20" s="354" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="K20" s="354"/>
       <c r="N20" s="359"/>
@@ -48432,19 +48438,19 @@
     </row>
     <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="183" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B21" s="183" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="F21" s="360"/>
       <c r="G21" s="183"/>
       <c r="H21" s="183"/>
       <c r="I21" s="89" t="s">
+        <v>1203</v>
+      </c>
+      <c r="J21" s="348" t="s">
         <v>1204</v>
-      </c>
-      <c r="J21" s="348" t="s">
-        <v>1205</v>
       </c>
       <c r="K21" s="348"/>
       <c r="N21" s="359"/>
@@ -48460,23 +48466,23 @@
     </row>
     <row r="22" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="183" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B22" s="183" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="F22" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G22" s="183" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H22" s="183"/>
       <c r="I22" s="89" t="s">
+        <v>1207</v>
+      </c>
+      <c r="J22" s="348" t="s">
         <v>1208</v>
-      </c>
-      <c r="J22" s="348" t="s">
-        <v>1209</v>
       </c>
       <c r="K22" s="348"/>
       <c r="N22" s="359"/>
@@ -48492,22 +48498,22 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="183" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B23" s="183" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
       <c r="H23" s="183"/>
       <c r="I23" s="89" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J23" s="354" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="K23" s="354" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="L23" s="89" t="s">
         <v>38</v>
@@ -48520,7 +48526,7 @@
       <c r="P23" s="183"/>
       <c r="Q23" s="183"/>
       <c r="R23" s="183" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S23" s="183"/>
       <c r="T23" s="183"/>
@@ -48530,22 +48536,22 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="183" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B24" s="183" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
       <c r="H24" s="183"/>
       <c r="I24" s="89" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J24" s="354" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="K24" s="354" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="L24" s="89" t="s">
         <v>38</v>
@@ -48558,7 +48564,7 @@
       <c r="P24" s="183"/>
       <c r="Q24" s="183"/>
       <c r="R24" s="183" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S24" s="183"/>
       <c r="T24" s="183"/>
@@ -48568,35 +48574,35 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="183" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B25" s="183" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
       <c r="H25" s="183"/>
       <c r="I25" s="89" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="J25" s="354" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="K25" s="354" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="L25" s="183" t="s">
         <v>38</v>
       </c>
       <c r="M25" s="89" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="N25" s="359"/>
       <c r="O25" s="183"/>
       <c r="P25" s="183"/>
       <c r="Q25" s="183"/>
       <c r="R25" s="183" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S25" s="183"/>
       <c r="T25" s="183"/>
@@ -48606,22 +48612,22 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="183" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B26" s="183" t="s">
         <v>1265</v>
-      </c>
-      <c r="B26" s="183" t="s">
-        <v>1266</v>
       </c>
       <c r="F26" s="183"/>
       <c r="G26" s="183"/>
       <c r="H26" s="183"/>
       <c r="I26" s="349" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="J26" s="354" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="K26" s="354" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="L26" s="349" t="s">
         <v>38</v>
@@ -48639,22 +48645,22 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="183" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B27" s="183" t="s">
         <v>1268</v>
-      </c>
-      <c r="B27" s="183" t="s">
-        <v>1269</v>
       </c>
       <c r="F27" s="183"/>
       <c r="G27" s="183"/>
       <c r="H27" s="183"/>
       <c r="I27" s="183" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="J27" s="348" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="K27" s="348" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="L27" s="183" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
fixed a bud for PAR
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20402"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEE97D6-D240-4F30-A99F-076C7EA16A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="SBE MicroCATs" sheetId="1" r:id="rId1"/>
@@ -58,12 +57,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,12 +91,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>ocean.gbg11</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000002000000}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000003000000}">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000004000000}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -204,12 +203,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -238,12 +237,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -272,12 +271,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1000-000001000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4515,13 +4514,13 @@
     <t>prdM</t>
   </si>
   <si>
-    <t>PAR/Irradiance, PAR/Irradiance, Biospherical/Lico, Biospherical/Licor</t>
+    <t>PAR/Irradiance, Biospherical/Licor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
@@ -5938,12 +5937,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Förklarande text 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlänk 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Förklarande text 2" xfId="4"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlänk 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="1602">
     <dxf>
@@ -17652,7 +17651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -23674,79 +23673,79 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>W26:W1048576 W1:W17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576 W18:W25</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$23</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$M:$M</xm:f>
           </x14:formula1>
@@ -23759,7 +23758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -24713,25 +24712,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -24744,7 +24743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -25594,25 +25593,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -25625,7 +25624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -27220,19 +27219,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$45</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -27245,7 +27244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -29120,31 +29119,31 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$3:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$N$2:$N$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
@@ -29157,7 +29156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -29169,7 +29168,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -33183,73 +33182,73 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0E00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>AA1:AA1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0E00-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
           <xm:sqref>Z1:Z1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej" xr:uid="{00000000-0002-0000-0E00-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej">
           <x14:formula1>
             <xm:f>Listor!$M$3:$M$7</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A:$A</xm:f>
           </x14:formula1>
@@ -33262,7 +33261,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -45076,19 +45075,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -45101,7 +45100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -46929,19 +46928,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -46954,7 +46953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -47525,13 +47524,13 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -48677,7 +48676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -50402,115 +50401,115 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="19">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W4 W6:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>W5:X5 V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>X1:X4 X6:X1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H13 H16:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I13 I16:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J13 J16:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K13 K16:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$40</xm:f>
           </x14:formula1>
           <xm:sqref>H14:H15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>I14:I15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$3:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J14:J15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$11:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K14:K15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000010000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>L1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000011000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000012000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -50523,7 +50522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -51925,19 +51924,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H38 H41:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>H39:H40</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0200-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
@@ -51950,7 +51949,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L107"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -53093,20 +53092,20 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F23" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J15 J18:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -53119,7 +53118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -54207,13 +54206,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H2 H17:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -54226,7 +54225,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -54885,7 +54884,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
@@ -54898,7 +54897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S381"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -57483,37 +57482,37 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0600-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$L$2:$L$3</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
@@ -57526,7 +57525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -59933,49 +59932,49 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -59988,7 +59987,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -60754,19 +60753,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
changed PAR unit in instruments.xlsx
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20416"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\ctd_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\utveckling\sharktools_dev\temp_working_dir\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6F9F59-1008-4D67-91B2-9730D1BE0B92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18"/>
+    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SBE MicroCATs" sheetId="1" r:id="rId1"/>
@@ -57,12 +58,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -91,12 +92,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ocean.gbg11</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -147,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000003000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000004000000}">
       <text>
         <r>
           <rPr>
@@ -203,12 +204,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -237,12 +238,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -271,12 +272,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nordström Maria</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -4181,12 +4182,6 @@
     <t>PAR_CTD</t>
   </si>
   <si>
-    <t>1.4x10e-5</t>
-  </si>
-  <si>
-    <t>1.4x10e-5 µE/(cm2 ·sec) to 0.5 µE/(cm2 ·sec)</t>
-  </si>
-  <si>
     <t>WET Labs</t>
   </si>
   <si>
@@ -4382,9 +4377,6 @@
     <t>ml/l</t>
   </si>
   <si>
-    <t>µE/(cm2 sec)</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -4515,12 +4507,21 @@
   </si>
   <si>
     <t>PAR/Irradiance, Biospherical/Licor</t>
+  </si>
+  <si>
+    <t>µE/(m2 sec)</t>
+  </si>
+  <si>
+    <t>0.14 µE/(m2 ·sec) to 5000 µE/(m2 ·sec)</t>
+  </si>
+  <si>
+    <t>0.14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
@@ -5937,12 +5938,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Förklarande text 2" xfId="4"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlänk 2" xfId="3"/>
+    <cellStyle name="Förklarande text 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlänk 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="1602">
     <dxf>
@@ -17651,7 +17652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -23673,79 +23674,79 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>W26:W1048576 W1:W17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576 W18:W25</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$23</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000B000000}">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>Listor!$M:$M</xm:f>
           </x14:formula1>
@@ -23758,7 +23759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -24712,25 +24713,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -24743,7 +24744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -25593,25 +25594,25 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -25624,7 +25625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -27219,19 +27220,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$45</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -27244,7 +27245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -29119,31 +29120,31 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$3:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$N$2:$N$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
@@ -29156,7 +29157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -29168,7 +29169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AD100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -33182,73 +33183,73 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0E00-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>AA1:AA1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000002000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000003000000}">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000004000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000005000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000006000000}">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000007000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0E00-000008000000}">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
           <xm:sqref>Z1:Z1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sensor finns ej" xr:uid="{00000000-0002-0000-0E00-000009000000}">
           <x14:formula1>
             <xm:f>Listor!$M$3:$M$7</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000A000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-00000B000000}">
           <x14:formula1>
             <xm:f>Listor!$A:$A</xm:f>
           </x14:formula1>
@@ -33261,7 +33262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -45075,19 +45076,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$27</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -45100,7 +45101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -46928,19 +46929,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -46953,7 +46954,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -47524,13 +47525,13 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -47556,7 +47557,7 @@
         <v>1099</v>
       </c>
       <c r="B1" s="345" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="C1" s="345" t="s">
         <v>390</v>
@@ -47583,7 +47584,7 @@
         <v>1106</v>
       </c>
       <c r="K1" s="345" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="L1" s="345" t="s">
         <v>1107</v>
@@ -47612,7 +47613,7 @@
         <v>1114</v>
       </c>
       <c r="B2" s="346" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C2" s="346" t="s">
         <v>1115</v>
@@ -47639,7 +47640,7 @@
         <v>1122</v>
       </c>
       <c r="K2" s="346" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="L2" s="346" t="s">
         <v>1123</v>
@@ -47668,7 +47669,7 @@
         <v>1130</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="F3" s="360"/>
       <c r="G3" s="183"/>
@@ -47680,7 +47681,7 @@
         <v>1132</v>
       </c>
       <c r="K3" s="348" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="L3" s="89" t="s">
         <v>38</v>
@@ -47706,7 +47707,7 @@
         <v>1135</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>1136</v>
@@ -47733,7 +47734,7 @@
         <v>1143</v>
       </c>
       <c r="K4" s="348" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="N4" s="359" t="s">
         <v>1144</v>
@@ -47759,7 +47760,7 @@
         <v>1135</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>1136</v>
@@ -47777,7 +47778,7 @@
         <v>1148</v>
       </c>
       <c r="H5" s="361" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="I5" s="349" t="s">
         <v>1142</v>
@@ -47786,7 +47787,7 @@
         <v>1143</v>
       </c>
       <c r="K5" s="348" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="N5" s="351"/>
       <c r="O5" s="352" t="s">
@@ -47812,7 +47813,7 @@
         <v>1152</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="F6" s="360" t="s">
         <v>1137</v>
@@ -47824,13 +47825,13 @@
         <v>1153</v>
       </c>
       <c r="I6" s="349" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="J6" s="354" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="K6" s="354" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="L6" s="355"/>
       <c r="M6" s="355"/>
@@ -47858,7 +47859,7 @@
         <v>1152</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="F7" s="360" t="s">
         <v>1137</v>
@@ -47867,16 +47868,16 @@
         <v>1148</v>
       </c>
       <c r="H7" s="361" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="I7" s="349" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="J7" s="354" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="K7" s="354" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="L7" s="356"/>
       <c r="N7" s="183"/>
@@ -47903,19 +47904,19 @@
         <v>1159</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="F8" s="360"/>
       <c r="G8" s="183"/>
       <c r="H8" s="359"/>
       <c r="I8" s="349" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="J8" s="348" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="K8" s="348" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="L8" s="89" t="s">
         <v>38</v>
@@ -47943,7 +47944,7 @@
         <v>1163</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="F9" s="360" t="s">
         <v>1137</v>
@@ -47952,16 +47953,16 @@
         <v>647</v>
       </c>
       <c r="H9" s="359" t="s">
-        <v>1277</v>
+        <v>1274</v>
       </c>
       <c r="I9" s="349" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="J9" s="348" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="K9" s="348" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="L9" s="350"/>
       <c r="M9" s="350"/>
@@ -47989,7 +47990,7 @@
         <v>1163</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>1288</v>
+        <v>1285</v>
       </c>
       <c r="F10" s="360" t="s">
         <v>1137</v>
@@ -47998,16 +47999,16 @@
         <v>1148</v>
       </c>
       <c r="H10" s="361" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="I10" s="349" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="J10" s="348" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="K10" s="348" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="L10" s="350"/>
       <c r="M10" s="356"/>
@@ -48032,10 +48033,10 @@
     </row>
     <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="F11" s="360" t="s">
         <v>1137</v>
@@ -48047,13 +48048,13 @@
         <v>1170</v>
       </c>
       <c r="I11" s="349" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="J11" s="348" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="K11" s="348" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="L11" s="350"/>
       <c r="M11" s="350"/>
@@ -48083,19 +48084,19 @@
         <v>1175</v>
       </c>
       <c r="B12" s="183" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="F12" s="360"/>
       <c r="G12" s="183"/>
       <c r="H12" s="359"/>
       <c r="I12" s="349" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="J12" s="348" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="K12" s="348" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="L12" s="89" t="s">
         <v>38</v>
@@ -48113,19 +48114,19 @@
     </row>
     <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="183" t="s">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="B13" s="183" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="F13" s="360" t="s">
         <v>1176</v>
       </c>
       <c r="G13" s="360" t="s">
-        <v>1287</v>
+        <v>1284</v>
       </c>
       <c r="H13" s="359" t="s">
-        <v>1285</v>
+        <v>1282</v>
       </c>
       <c r="I13" s="89" t="s">
         <v>1177</v>
@@ -48134,15 +48135,15 @@
         <v>1178</v>
       </c>
       <c r="K13" s="348" t="s">
-        <v>1246</v>
+        <v>1288</v>
       </c>
       <c r="L13" s="350"/>
       <c r="M13" s="350"/>
       <c r="N13" s="359" t="s">
-        <v>1179</v>
+        <v>1290</v>
       </c>
       <c r="O13" s="183" t="s">
-        <v>1180</v>
+        <v>1289</v>
       </c>
       <c r="P13" s="183"/>
       <c r="Q13" s="183"/>
@@ -48155,37 +48156,37 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="183" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B14" s="183" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="F14" s="183" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="G14" s="183" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="H14" s="359" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="J14" s="354" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="K14" s="354" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="N14" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O14" s="183" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="P14" s="183" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="Q14" s="183">
         <v>8</v>
@@ -48199,37 +48200,37 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="183" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="B15" s="183" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="F15" s="183" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="G15" s="183" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="H15" s="359" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="I15" s="53" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="J15" s="354" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="K15" s="354" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="N15" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O15" s="183" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="P15" s="183" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="Q15" s="183">
         <v>8</v>
@@ -48243,37 +48244,37 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="183" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B16" s="183" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="F16" s="183" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="G16" s="183" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="H16" s="359" t="s">
         <v>235</v>
       </c>
       <c r="I16" s="53" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="J16" s="354" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="K16" s="354" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="N16" s="359" t="s">
         <v>1144</v>
       </c>
       <c r="O16" s="183" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="P16" s="183" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="Q16" s="183">
         <v>8</v>
@@ -48290,34 +48291,34 @@
         <v>574</v>
       </c>
       <c r="B17" s="183" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="F17" s="183" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="G17" s="183" t="s">
         <v>571</v>
       </c>
       <c r="H17" s="359" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J17" s="354" t="s">
+        <v>1191</v>
+      </c>
+      <c r="K17" s="354" t="s">
+        <v>1248</v>
+      </c>
+      <c r="N17" s="359" t="s">
+        <v>1192</v>
+      </c>
+      <c r="O17" s="183" t="s">
         <v>1193</v>
       </c>
-      <c r="K17" s="354" t="s">
-        <v>1251</v>
-      </c>
-      <c r="N17" s="359" t="s">
+      <c r="P17" s="183" t="s">
         <v>1194</v>
-      </c>
-      <c r="O17" s="183" t="s">
-        <v>1195</v>
-      </c>
-      <c r="P17" s="183" t="s">
-        <v>1196</v>
       </c>
       <c r="Q17" s="183"/>
       <c r="R17" s="183"/>
@@ -48332,7 +48333,7 @@
         <v>574</v>
       </c>
       <c r="B18" s="183" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="F18" s="183" t="s">
         <v>712</v>
@@ -48341,25 +48342,25 @@
         <v>713</v>
       </c>
       <c r="H18" s="359" t="s">
-        <v>1282</v>
+        <v>1279</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J18" s="354" t="s">
+        <v>1191</v>
+      </c>
+      <c r="K18" s="354" t="s">
+        <v>1248</v>
+      </c>
+      <c r="N18" s="359" t="s">
+        <v>1192</v>
+      </c>
+      <c r="O18" s="183" t="s">
         <v>1193</v>
       </c>
-      <c r="K18" s="354" t="s">
-        <v>1251</v>
-      </c>
-      <c r="N18" s="359" t="s">
+      <c r="P18" s="183" t="s">
         <v>1194</v>
-      </c>
-      <c r="O18" s="183" t="s">
-        <v>1195</v>
-      </c>
-      <c r="P18" s="183" t="s">
-        <v>1196</v>
       </c>
       <c r="Q18" s="183"/>
       <c r="R18" s="183"/>
@@ -48371,35 +48372,35 @@
     </row>
     <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="183" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="B19" s="183" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="F19" s="360"/>
       <c r="G19" s="183"/>
       <c r="H19" s="183"/>
       <c r="I19" s="53" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="J19" s="354" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="K19" s="354" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="L19" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M19" s="89" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="N19" s="359"/>
       <c r="O19" s="183"/>
       <c r="P19" s="183"/>
       <c r="Q19" s="183"/>
       <c r="R19" s="183" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="S19" s="183"/>
       <c r="T19" s="183"/>
@@ -48409,19 +48410,19 @@
     </row>
     <row r="20" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="183" t="s">
-        <v>1281</v>
+        <v>1278</v>
       </c>
       <c r="B20" s="183" t="s">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="F20" s="360"/>
       <c r="G20" s="183"/>
       <c r="H20" s="183"/>
       <c r="I20" s="53" t="s">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="J20" s="354" t="s">
-        <v>1278</v>
+        <v>1275</v>
       </c>
       <c r="K20" s="354"/>
       <c r="N20" s="359"/>
@@ -48437,19 +48438,19 @@
     </row>
     <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="183" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="B21" s="183" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="F21" s="360"/>
       <c r="G21" s="183"/>
       <c r="H21" s="183"/>
       <c r="I21" s="89" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="J21" s="348" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="K21" s="348"/>
       <c r="N21" s="359"/>
@@ -48465,23 +48466,23 @@
     </row>
     <row r="22" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="183" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B22" s="183" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="F22" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G22" s="183" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="H22" s="183"/>
       <c r="I22" s="89" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="J22" s="348" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="K22" s="348"/>
       <c r="N22" s="359"/>
@@ -48497,22 +48498,22 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="183" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B23" s="183" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
       <c r="H23" s="183"/>
       <c r="I23" s="89" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="J23" s="354" t="s">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="K23" s="354" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="L23" s="89" t="s">
         <v>38</v>
@@ -48525,7 +48526,7 @@
       <c r="P23" s="183"/>
       <c r="Q23" s="183"/>
       <c r="R23" s="183" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="S23" s="183"/>
       <c r="T23" s="183"/>
@@ -48535,22 +48536,22 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="183" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B24" s="183" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
       <c r="H24" s="183"/>
       <c r="I24" s="89" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="J24" s="354" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="K24" s="354" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="L24" s="89" t="s">
         <v>38</v>
@@ -48563,7 +48564,7 @@
       <c r="P24" s="183"/>
       <c r="Q24" s="183"/>
       <c r="R24" s="183" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="S24" s="183"/>
       <c r="T24" s="183"/>
@@ -48573,35 +48574,35 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="183" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="B25" s="183" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
       <c r="H25" s="183"/>
       <c r="I25" s="89" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="J25" s="354" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="K25" s="354" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="L25" s="183" t="s">
         <v>38</v>
       </c>
       <c r="M25" s="89" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="N25" s="359"/>
       <c r="O25" s="183"/>
       <c r="P25" s="183"/>
       <c r="Q25" s="183"/>
       <c r="R25" s="183" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="S25" s="183"/>
       <c r="T25" s="183"/>
@@ -48611,22 +48612,22 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="183" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="B26" s="183" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="F26" s="183"/>
       <c r="G26" s="183"/>
       <c r="H26" s="183"/>
       <c r="I26" s="349" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="J26" s="354" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="K26" s="354" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="L26" s="349" t="s">
         <v>38</v>
@@ -48644,22 +48645,22 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="183" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="B27" s="183" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="F27" s="183"/>
       <c r="G27" s="183"/>
       <c r="H27" s="183"/>
       <c r="I27" s="183" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="J27" s="348" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="K27" s="348" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="L27" s="183" t="s">
         <v>38</v>
@@ -48676,7 +48677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -50401,115 +50402,115 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="19">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>W1:W4 W6:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>W5:X5 V1:V1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>X1:X4 X6:X1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$38</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H13 H16:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I13 I16:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$5:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J13 J16:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$13:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K13 K16:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>'SBE Dissolved Oxygen Sensors'!$D$3:$D$40</xm:f>
           </x14:formula1>
           <xm:sqref>H14:H15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>'SBE Pumps'!$D$3:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>I14:I15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$3:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>J14:J15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>'SBE T&amp;C-sensors'!$D$11:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>K14:K15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Listor!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>U1:U1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$47</xm:f>
           </x14:formula1>
           <xm:sqref>O1:O1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000010000000}">
           <x14:formula1>
             <xm:f>WETLabs!$D$3:$D$25</xm:f>
           </x14:formula1>
           <xm:sqref>L1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000011000000}">
           <x14:formula1>
             <xm:f>Listor!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000012000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -50522,7 +50523,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -51924,19 +51925,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H38 H41:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>H39:H40</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number MicroCAT" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>'SBE MicroCATs'!$E$3:$E$104</xm:f>
           </x14:formula1>
@@ -51949,7 +51950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L107"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -53092,20 +53093,20 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1"/>
+    <hyperlink ref="F23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J15 J18:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -53118,7 +53119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -54206,13 +54207,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$12</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H2 H17:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
@@ -54225,7 +54226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -54884,7 +54885,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$7</xm:f>
           </x14:formula1>
@@ -54897,7 +54898,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S381"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -57482,37 +57483,37 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Non Valid Serial Number SeaCAT" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>'SBE SeaCATs'!$D$3:$D$15</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$A$2:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$L$2:$L$3</xm:f>
           </x14:formula1>
           <xm:sqref>N1:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$D:$D</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000005000000}">
           <x14:formula1>
             <xm:f>Listor!$C:$C</xm:f>
           </x14:formula1>
@@ -57525,7 +57526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -59932,49 +59933,49 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>R1:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000003000000}">
           <x14:formula1>
             <xm:f>Listor!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000004000000}">
           <x14:formula1>
             <xm:f>Listor!$K$2:$K$3</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000005000000}">
           <x14:formula1>
             <xm:f>Listor!$H$2:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>Q1:Q1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000006000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000007000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>
@@ -59987,7 +59988,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -60753,19 +60754,19 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>Listor!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
           <x14:formula1>
             <xm:f>Listor!$C$2:$C$42</xm:f>
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000002000000}">
           <x14:formula1>
             <xm:f>Listor!$B$2:$B$10</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Added SLUs New SBE19 sensors and updated some missing sensornr/fields
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\utveckling\sharktools_dev\temp_working_dir\ctd_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6F9F59-1008-4D67-91B2-9730D1BE0B92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71D8F75-3A5A-4ED5-B374-3E5457A66E18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="1300">
   <si>
     <t>Model</t>
   </si>
@@ -4068,9 +4068,6 @@
     <t>Digiquartz 8000-series</t>
   </si>
   <si>
-    <t>1044, 1387, 0745</t>
-  </si>
-  <si>
     <t>Tryck</t>
   </si>
   <si>
@@ -4104,9 +4101,6 @@
     <t>Conductivity</t>
   </si>
   <si>
-    <t>3941, 3943, 2997, 2994, 4829, 4824</t>
-  </si>
-  <si>
     <t>0.0-7.0 S/m</t>
   </si>
   <si>
@@ -4155,9 +4149,6 @@
     <t>Typical Stability: 0.0003 S/m per month. Resolution: 0.00005 S/m typical</t>
   </si>
   <si>
-    <t>0732, 1243, 0732, 2126, 2127, 3823, 3829</t>
-  </si>
-  <si>
     <t>0.1</t>
   </si>
   <si>
@@ -4467,9 +4458,6 @@
     <t>SIGMA_THETA_CTD</t>
   </si>
   <si>
-    <t>5351, 5355, 6378, 6384, 4361, 4387</t>
-  </si>
-  <si>
     <t>SCAN_BIN_CTD</t>
   </si>
   <si>
@@ -4488,15 +4476,6 @@
     <t>53447, 1251</t>
   </si>
   <si>
-    <t>6164, 6929</t>
-  </si>
-  <si>
-    <t>70374, 70711, 70397</t>
-  </si>
-  <si>
-    <t>FLNTURTD-2288, FLNTURT-115, FLNTURT-1899, FLNTURT-2470</t>
-  </si>
-  <si>
     <t>QSP-2000, QSP-2350</t>
   </si>
   <si>
@@ -4516,6 +4495,54 @@
   </si>
   <si>
     <t>0.14</t>
+  </si>
+  <si>
+    <t>1044, 1387, 0745, 1464</t>
+  </si>
+  <si>
+    <t>3941, 3943, 2997, 2994, 4829, 4824, 5060</t>
+  </si>
+  <si>
+    <t>5351, 5355, 6378, 6384, 4361, 4387, 6596</t>
+  </si>
+  <si>
+    <t>Time, NMEA</t>
+  </si>
+  <si>
+    <t>timeQ</t>
+  </si>
+  <si>
+    <t>Scan tid (sekunder sedan 2000-01-01)</t>
+  </si>
+  <si>
+    <t>SCAN_TIME_CTD</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>Time, Elapsed</t>
+  </si>
+  <si>
+    <t>timeS</t>
+  </si>
+  <si>
+    <t>Förfluten tid (sekunder sedan system upload time)</t>
+  </si>
+  <si>
+    <t>SCAN_TIME_ELAP_CTD</t>
+  </si>
+  <si>
+    <t>6164, 6929, 8438</t>
+  </si>
+  <si>
+    <t>FLNTURTD-2288, FLNTURT-115, FLNTURT-1899, FLNTURT-2470, FLNTURT-9297</t>
+  </si>
+  <si>
+    <t>0732, 1243, 0732, 2126, 2127, 3823, 3829, 4152, 4649</t>
+  </si>
+  <si>
+    <t>70374, 70711, 70397, 2140, 2112, 70785</t>
   </si>
 </sst>
 </file>
@@ -47526,12 +47553,12 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:W27"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -47557,7 +47584,7 @@
         <v>1099</v>
       </c>
       <c r="B1" s="345" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="C1" s="345" t="s">
         <v>390</v>
@@ -47584,7 +47611,7 @@
         <v>1106</v>
       </c>
       <c r="K1" s="345" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="L1" s="345" t="s">
         <v>1107</v>
@@ -47613,7 +47640,7 @@
         <v>1114</v>
       </c>
       <c r="B2" s="346" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="C2" s="346" t="s">
         <v>1115</v>
@@ -47640,7 +47667,7 @@
         <v>1122</v>
       </c>
       <c r="K2" s="346" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="L2" s="346" t="s">
         <v>1123</v>
@@ -47669,7 +47696,7 @@
         <v>1130</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="F3" s="360"/>
       <c r="G3" s="183"/>
@@ -47681,7 +47708,7 @@
         <v>1132</v>
       </c>
       <c r="K3" s="348" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="L3" s="89" t="s">
         <v>38</v>
@@ -47707,7 +47734,7 @@
         <v>1135</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>1136</v>
@@ -47725,25 +47752,25 @@
         <v>1140</v>
       </c>
       <c r="H4" s="359" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I4" s="349" t="s">
         <v>1141</v>
       </c>
-      <c r="I4" s="349" t="s">
+      <c r="J4" s="348" t="s">
         <v>1142</v>
       </c>
-      <c r="J4" s="348" t="s">
+      <c r="K4" s="348" t="s">
+        <v>1236</v>
+      </c>
+      <c r="N4" s="359" t="s">
         <v>1143</v>
       </c>
-      <c r="K4" s="348" t="s">
-        <v>1239</v>
-      </c>
-      <c r="N4" s="359" t="s">
+      <c r="O4" s="183" t="s">
         <v>1144</v>
       </c>
-      <c r="O4" s="183" t="s">
+      <c r="P4" s="183" t="s">
         <v>1145</v>
-      </c>
-      <c r="P4" s="183" t="s">
-        <v>1146</v>
       </c>
       <c r="Q4" s="183">
         <v>24</v>
@@ -47760,7 +47787,7 @@
         <v>1135</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>1286</v>
+        <v>1279</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>1136</v>
@@ -47769,38 +47796,38 @@
         <v>1137</v>
       </c>
       <c r="E5" s="89" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F5" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G5" s="183" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="H5" s="361" t="s">
-        <v>1281</v>
+        <v>1296</v>
       </c>
       <c r="I5" s="349" t="s">
+        <v>1141</v>
+      </c>
+      <c r="J5" s="348" t="s">
         <v>1142</v>
       </c>
-      <c r="J5" s="348" t="s">
-        <v>1143</v>
-      </c>
       <c r="K5" s="348" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="N5" s="351"/>
       <c r="O5" s="352" t="s">
+        <v>1148</v>
+      </c>
+      <c r="P5" s="351" t="s">
         <v>1149</v>
-      </c>
-      <c r="P5" s="351" t="s">
-        <v>1150</v>
       </c>
       <c r="Q5" s="352">
         <v>4</v>
       </c>
       <c r="R5" s="353" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="S5" s="183"/>
       <c r="T5" s="183"/>
@@ -47810,10 +47837,10 @@
     </row>
     <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="89" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="F6" s="360" t="s">
         <v>1137</v>
@@ -47822,27 +47849,27 @@
         <v>199</v>
       </c>
       <c r="H6" s="359" t="s">
-        <v>1153</v>
+        <v>1285</v>
       </c>
       <c r="I6" s="349" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="J6" s="354" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="K6" s="354" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="L6" s="355"/>
       <c r="M6" s="355"/>
       <c r="N6" s="359" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="O6" s="183" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="P6" s="183" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="Q6" s="183">
         <v>24</v>
@@ -47856,42 +47883,42 @@
     </row>
     <row r="7" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="F7" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G7" s="183" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="H7" s="361" t="s">
-        <v>1281</v>
+        <v>1296</v>
       </c>
       <c r="I7" s="349" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="J7" s="354" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="K7" s="354" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="L7" s="356"/>
       <c r="N7" s="183"/>
       <c r="O7" s="356" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="P7" s="356" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="Q7" s="357">
         <v>4</v>
       </c>
       <c r="R7" s="183" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="S7" s="183"/>
       <c r="T7" s="183"/>
@@ -47901,37 +47928,37 @@
     </row>
     <row r="8" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="89" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="F8" s="360"/>
       <c r="G8" s="183"/>
       <c r="H8" s="359"/>
       <c r="I8" s="349" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="J8" s="348" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="K8" s="348" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="L8" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M8" s="89" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="N8" s="359" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="O8" s="362"/>
       <c r="P8" s="362"/>
       <c r="Q8" s="362"/>
       <c r="R8" s="183" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="S8" s="183"/>
       <c r="T8" s="183"/>
@@ -47941,10 +47968,10 @@
     </row>
     <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="F9" s="360" t="s">
         <v>1137</v>
@@ -47953,27 +47980,27 @@
         <v>647</v>
       </c>
       <c r="H9" s="359" t="s">
-        <v>1274</v>
+        <v>1286</v>
       </c>
       <c r="I9" s="349" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="J9" s="348" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="K9" s="348" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="L9" s="350"/>
       <c r="M9" s="350"/>
       <c r="N9" s="359" t="s">
+        <v>1162</v>
+      </c>
+      <c r="O9" s="363" t="s">
+        <v>1163</v>
+      </c>
+      <c r="P9" s="183" t="s">
         <v>1164</v>
-      </c>
-      <c r="O9" s="363" t="s">
-        <v>1165</v>
-      </c>
-      <c r="P9" s="183" t="s">
-        <v>1166</v>
       </c>
       <c r="Q9" s="183">
         <v>24</v>
@@ -47987,43 +48014,43 @@
     </row>
     <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="89" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>1285</v>
+        <v>1278</v>
       </c>
       <c r="F10" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G10" s="183" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="H10" s="361" t="s">
-        <v>1281</v>
+        <v>1296</v>
       </c>
       <c r="I10" s="349" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="J10" s="348" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="K10" s="348" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="L10" s="350"/>
       <c r="M10" s="356"/>
       <c r="N10" s="183"/>
       <c r="O10" s="356" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="P10" s="356" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="Q10" s="357">
         <v>4</v>
       </c>
       <c r="R10" s="183" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="S10" s="183"/>
       <c r="T10" s="183"/>
@@ -48033,10 +48060,10 @@
     </row>
     <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="89" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="F11" s="360" t="s">
         <v>1137</v>
@@ -48045,33 +48072,33 @@
         <v>174</v>
       </c>
       <c r="H11" s="359" t="s">
-        <v>1170</v>
+        <v>1298</v>
       </c>
       <c r="I11" s="349" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="J11" s="348" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="K11" s="348" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="L11" s="350"/>
       <c r="M11" s="350"/>
       <c r="N11" s="359" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="O11" s="183" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="P11" s="183" t="s">
         <v>566</v>
       </c>
       <c r="Q11" s="183" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="R11" s="183" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="S11" s="183"/>
       <c r="T11" s="183"/>
@@ -48081,22 +48108,22 @@
     </row>
     <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="183" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="B12" s="183" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="F12" s="360"/>
       <c r="G12" s="183"/>
       <c r="H12" s="359"/>
       <c r="I12" s="349" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="J12" s="348" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="K12" s="348" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="L12" s="89" t="s">
         <v>38</v>
@@ -48114,36 +48141,36 @@
     </row>
     <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="183" t="s">
-        <v>1287</v>
+        <v>1280</v>
       </c>
       <c r="B13" s="183" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="F13" s="360" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="G13" s="360" t="s">
-        <v>1284</v>
+        <v>1277</v>
       </c>
       <c r="H13" s="359" t="s">
-        <v>1282</v>
+        <v>1299</v>
       </c>
       <c r="I13" s="89" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="J13" s="348" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="K13" s="348" t="s">
-        <v>1288</v>
+        <v>1281</v>
       </c>
       <c r="L13" s="350"/>
       <c r="M13" s="350"/>
       <c r="N13" s="359" t="s">
-        <v>1290</v>
+        <v>1283</v>
       </c>
       <c r="O13" s="183" t="s">
-        <v>1289</v>
+        <v>1282</v>
       </c>
       <c r="P13" s="183"/>
       <c r="Q13" s="183"/>
@@ -48156,37 +48183,37 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="183" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="B14" s="183" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="F14" s="183" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G14" s="183" t="s">
+        <v>1177</v>
+      </c>
+      <c r="H14" s="359" t="s">
+        <v>1297</v>
+      </c>
+      <c r="I14" s="53" t="s">
+        <v>1256</v>
+      </c>
+      <c r="J14" s="354" t="s">
+        <v>1255</v>
+      </c>
+      <c r="K14" s="354" t="s">
+        <v>1242</v>
+      </c>
+      <c r="N14" s="359" t="s">
+        <v>1143</v>
+      </c>
+      <c r="O14" s="183" t="s">
+        <v>1178</v>
+      </c>
+      <c r="P14" s="183" t="s">
         <v>1179</v>
-      </c>
-      <c r="G14" s="183" t="s">
-        <v>1180</v>
-      </c>
-      <c r="H14" s="359" t="s">
-        <v>1283</v>
-      </c>
-      <c r="I14" s="53" t="s">
-        <v>1259</v>
-      </c>
-      <c r="J14" s="354" t="s">
-        <v>1258</v>
-      </c>
-      <c r="K14" s="354" t="s">
-        <v>1245</v>
-      </c>
-      <c r="N14" s="359" t="s">
-        <v>1144</v>
-      </c>
-      <c r="O14" s="183" t="s">
-        <v>1181</v>
-      </c>
-      <c r="P14" s="183" t="s">
-        <v>1182</v>
       </c>
       <c r="Q14" s="183">
         <v>8</v>
@@ -48200,37 +48227,37 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="183" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="B15" s="183" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="F15" s="183" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="G15" s="183" t="s">
+        <v>1177</v>
+      </c>
+      <c r="H15" s="359" t="s">
+        <v>1297</v>
+      </c>
+      <c r="I15" s="53" t="s">
         <v>1180</v>
       </c>
-      <c r="H15" s="359" t="s">
-        <v>1283</v>
-      </c>
-      <c r="I15" s="53" t="s">
+      <c r="J15" s="354" t="s">
+        <v>1181</v>
+      </c>
+      <c r="K15" s="354" t="s">
+        <v>1243</v>
+      </c>
+      <c r="N15" s="359" t="s">
+        <v>1143</v>
+      </c>
+      <c r="O15" s="183" t="s">
+        <v>1182</v>
+      </c>
+      <c r="P15" s="183" t="s">
         <v>1183</v>
-      </c>
-      <c r="J15" s="354" t="s">
-        <v>1184</v>
-      </c>
-      <c r="K15" s="354" t="s">
-        <v>1246</v>
-      </c>
-      <c r="N15" s="359" t="s">
-        <v>1144</v>
-      </c>
-      <c r="O15" s="183" t="s">
-        <v>1185</v>
-      </c>
-      <c r="P15" s="183" t="s">
-        <v>1186</v>
       </c>
       <c r="Q15" s="183">
         <v>8</v>
@@ -48244,37 +48271,37 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="183" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="B16" s="183" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="F16" s="183" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="G16" s="183" t="s">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="H16" s="359" t="s">
         <v>235</v>
       </c>
       <c r="I16" s="53" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="J16" s="354" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="K16" s="354" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="N16" s="359" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="O16" s="183" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="P16" s="183" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="Q16" s="183">
         <v>8</v>
@@ -48291,34 +48318,34 @@
         <v>574</v>
       </c>
       <c r="B17" s="183" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="F17" s="183" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="G17" s="183" t="s">
         <v>571</v>
       </c>
       <c r="H17" s="359" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J17" s="354" t="s">
+        <v>1188</v>
+      </c>
+      <c r="K17" s="354" t="s">
+        <v>1245</v>
+      </c>
+      <c r="N17" s="359" t="s">
+        <v>1189</v>
+      </c>
+      <c r="O17" s="183" t="s">
+        <v>1190</v>
+      </c>
+      <c r="P17" s="183" t="s">
         <v>1191</v>
-      </c>
-      <c r="K17" s="354" t="s">
-        <v>1248</v>
-      </c>
-      <c r="N17" s="359" t="s">
-        <v>1192</v>
-      </c>
-      <c r="O17" s="183" t="s">
-        <v>1193</v>
-      </c>
-      <c r="P17" s="183" t="s">
-        <v>1194</v>
       </c>
       <c r="Q17" s="183"/>
       <c r="R17" s="183"/>
@@ -48333,7 +48360,7 @@
         <v>574</v>
       </c>
       <c r="B18" s="183" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="F18" s="183" t="s">
         <v>712</v>
@@ -48342,25 +48369,25 @@
         <v>713</v>
       </c>
       <c r="H18" s="359" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>574</v>
       </c>
       <c r="J18" s="354" t="s">
+        <v>1188</v>
+      </c>
+      <c r="K18" s="354" t="s">
+        <v>1245</v>
+      </c>
+      <c r="N18" s="359" t="s">
+        <v>1189</v>
+      </c>
+      <c r="O18" s="183" t="s">
+        <v>1190</v>
+      </c>
+      <c r="P18" s="183" t="s">
         <v>1191</v>
-      </c>
-      <c r="K18" s="354" t="s">
-        <v>1248</v>
-      </c>
-      <c r="N18" s="359" t="s">
-        <v>1192</v>
-      </c>
-      <c r="O18" s="183" t="s">
-        <v>1193</v>
-      </c>
-      <c r="P18" s="183" t="s">
-        <v>1194</v>
       </c>
       <c r="Q18" s="183"/>
       <c r="R18" s="183"/>
@@ -48372,35 +48399,35 @@
     </row>
     <row r="19" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="183" t="s">
-        <v>1195</v>
+        <v>1192</v>
       </c>
       <c r="B19" s="183" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="F19" s="360"/>
       <c r="G19" s="183"/>
       <c r="H19" s="183"/>
       <c r="I19" s="53" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="J19" s="354" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="K19" s="354" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="L19" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M19" s="89" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="N19" s="359"/>
       <c r="O19" s="183"/>
       <c r="P19" s="183"/>
       <c r="Q19" s="183"/>
       <c r="R19" s="183" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="S19" s="183"/>
       <c r="T19" s="183"/>
@@ -48410,19 +48437,19 @@
     </row>
     <row r="20" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="183" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="B20" s="183" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="F20" s="360"/>
       <c r="G20" s="183"/>
       <c r="H20" s="183"/>
       <c r="I20" s="53" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="J20" s="354" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="K20" s="354"/>
       <c r="N20" s="359"/>
@@ -48438,19 +48465,19 @@
     </row>
     <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="183" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="B21" s="183" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="F21" s="360"/>
       <c r="G21" s="183"/>
       <c r="H21" s="183"/>
       <c r="I21" s="89" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="J21" s="348" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="K21" s="348"/>
       <c r="N21" s="359"/>
@@ -48466,23 +48493,23 @@
     </row>
     <row r="22" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="183" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="B22" s="183" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="F22" s="360" t="s">
         <v>1137</v>
       </c>
       <c r="G22" s="183" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="H22" s="183"/>
       <c r="I22" s="89" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="J22" s="348" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="K22" s="348"/>
       <c r="N22" s="359"/>
@@ -48498,35 +48525,35 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="183" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B23" s="183" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="F23" s="183"/>
       <c r="G23" s="183"/>
       <c r="H23" s="183"/>
       <c r="I23" s="89" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="J23" s="354" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="K23" s="354" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="L23" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M23" s="89" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="N23" s="359"/>
       <c r="O23" s="183"/>
       <c r="P23" s="183"/>
       <c r="Q23" s="183"/>
       <c r="R23" s="183" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="S23" s="183"/>
       <c r="T23" s="183"/>
@@ -48536,35 +48563,35 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="183" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B24" s="183" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="F24" s="183"/>
       <c r="G24" s="183"/>
       <c r="H24" s="183"/>
       <c r="I24" s="89" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="J24" s="354" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="K24" s="354" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="L24" s="89" t="s">
         <v>38</v>
       </c>
       <c r="M24" s="89" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="N24" s="359"/>
       <c r="O24" s="183"/>
       <c r="P24" s="183"/>
       <c r="Q24" s="183"/>
       <c r="R24" s="183" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="S24" s="183"/>
       <c r="T24" s="183"/>
@@ -48574,35 +48601,35 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="183" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="B25" s="183" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="F25" s="183"/>
       <c r="G25" s="183"/>
       <c r="H25" s="183"/>
       <c r="I25" s="89" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="J25" s="354" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="K25" s="354" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="L25" s="183" t="s">
         <v>38</v>
       </c>
       <c r="M25" s="89" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="N25" s="359"/>
       <c r="O25" s="183"/>
       <c r="P25" s="183"/>
       <c r="Q25" s="183"/>
       <c r="R25" s="183" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="S25" s="183"/>
       <c r="T25" s="183"/>
@@ -48612,22 +48639,22 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="183" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="B26" s="183" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="F26" s="183"/>
       <c r="G26" s="183"/>
       <c r="H26" s="183"/>
       <c r="I26" s="349" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="J26" s="354" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="K26" s="354" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="L26" s="349" t="s">
         <v>38</v>
@@ -48645,22 +48672,22 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="183" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="B27" s="183" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="F27" s="183"/>
       <c r="G27" s="183"/>
       <c r="H27" s="183"/>
       <c r="I27" s="183" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="J27" s="348" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="K27" s="348" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="L27" s="183" t="s">
         <v>38</v>
@@ -48669,6 +48696,46 @@
       <c r="O27" s="183"/>
       <c r="P27" s="183"/>
       <c r="Q27" s="183"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A28" s="89" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B28" s="89" t="s">
+        <v>1288</v>
+      </c>
+      <c r="I28" s="183" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J28" s="354" t="s">
+        <v>1290</v>
+      </c>
+      <c r="K28" s="354" t="s">
+        <v>1291</v>
+      </c>
+      <c r="L28" s="183" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A29" s="89" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B29" s="89" t="s">
+        <v>1293</v>
+      </c>
+      <c r="I29" s="183" t="s">
+        <v>1294</v>
+      </c>
+      <c r="J29" s="354" t="s">
+        <v>1295</v>
+      </c>
+      <c r="K29" s="354" t="s">
+        <v>1291</v>
+      </c>
+      <c r="L29" s="183" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
La till saknad syresensor i instrument.xlsx och uppdaterat SOC x2
</commit_message>
<xml_diff>
--- a/Instruments.xlsx
+++ b/Instruments.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20416"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svea_ctd\ctd_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCADB658-FDB3-4470-B4DA-7A4904764015}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-30" windowWidth="18900" windowHeight="7125" tabRatio="866"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor_info" sheetId="19" r:id="rId1"/>
@@ -655,16 +654,16 @@
     <t>FLNTURTD-2288, FLNTURT-115, FLNTURT-1899, FLNTURT-2470, FLNTURT-9297</t>
   </si>
   <si>
-    <t>0732, 1243, 0732, 2126, 2127, 3823, 3829, 4152, 4649</t>
-  </si>
-  <si>
     <t>70374, 70711, 70397, 2140, 2112, 70785</t>
+  </si>
+  <si>
+    <t>0732, 1243, 0732, 2126, 2127, 3823, 3829, 4152, 4649, 1823</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -841,11 +840,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Förklarande text 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Hyperlänk 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Förklarande text 2" xfId="3"/>
+    <cellStyle name="Hyperlänk 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1339,13 +1338,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1357,7 +1356,7 @@
     <col min="5" max="5" width="18.875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.75" style="2" customWidth="1"/>
     <col min="7" max="7" width="18.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="53" style="2" customWidth="1"/>
     <col min="9" max="9" width="24.375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.5" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="2" customWidth="1"/>
@@ -1859,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>128</v>
@@ -1940,7 +1939,7 @@
         <v>189</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>86</v>

</xml_diff>